<commit_message>
241118_1036am_updated CCA report time horizons
</commit_message>
<xml_diff>
--- a/ACCU PnL Output.xlsx
+++ b/ACCU PnL Output.xlsx
@@ -479,16 +479,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-694212</v>
+        <v>-834512</v>
       </c>
       <c r="C2" t="n">
-        <v>-313891.0835269513</v>
+        <v>-563308.1341747127</v>
       </c>
       <c r="D2" t="n">
-        <v>1074150.927734752</v>
+        <v>1085569.534795035</v>
       </c>
       <c r="E2" t="n">
-        <v>66047.84420780092</v>
+        <v>-312250.5993796773</v>
       </c>
     </row>
     <row r="3">
@@ -496,16 +496,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-660182</v>
+        <v>-797257</v>
       </c>
       <c r="C3" t="n">
-        <v>-298198.1377032989</v>
+        <v>-537006.0408834483</v>
       </c>
       <c r="D3" t="n">
-        <v>975378.4422311699</v>
+        <v>986674.7354647927</v>
       </c>
       <c r="E3" t="n">
-        <v>16998.30452787108</v>
+        <v>-347588.3054186557</v>
       </c>
     </row>
     <row r="4">
@@ -513,16 +513,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-626152</v>
+        <v>-760002</v>
       </c>
       <c r="C4" t="n">
-        <v>-282505.1918796464</v>
+        <v>-510703.9475921839</v>
       </c>
       <c r="D4" t="n">
-        <v>877805.6755908101</v>
+        <v>888905.0619839121</v>
       </c>
       <c r="E4" t="n">
-        <v>-30851.51628883625</v>
+        <v>-381800.8856082718</v>
       </c>
     </row>
     <row r="5">
@@ -530,16 +530,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-592122</v>
+        <v>-722747</v>
       </c>
       <c r="C5" t="n">
-        <v>-266812.246055994</v>
+        <v>-484401.8543009196</v>
       </c>
       <c r="D5" t="n">
-        <v>782171.8844634427</v>
+        <v>792986.9898404942</v>
       </c>
       <c r="E5" t="n">
-        <v>-76762.36159255123</v>
+        <v>-414161.8644604255</v>
       </c>
     </row>
     <row r="6">
@@ -547,16 +547,16 @@
         <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>-558092</v>
+        <v>-685492</v>
       </c>
       <c r="C6" t="n">
-        <v>-251119.3002323415</v>
+        <v>-458099.7610096553</v>
       </c>
       <c r="D6" t="n">
-        <v>689402.899940727</v>
+        <v>699846.2195708972</v>
       </c>
       <c r="E6" t="n">
-        <v>-119808.4002916145</v>
+        <v>-443745.541438758</v>
       </c>
     </row>
     <row r="7">
@@ -564,16 +564,16 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>-524061.9999999999</v>
+        <v>-648237</v>
       </c>
       <c r="C7" t="n">
-        <v>-235426.3544086891</v>
+        <v>-431797.6677183909</v>
       </c>
       <c r="D7" t="n">
-        <v>600543.9863173725</v>
+        <v>610543.4018159758</v>
       </c>
       <c r="E7" t="n">
-        <v>-158944.3680913165</v>
+        <v>-469491.2659024152</v>
       </c>
     </row>
     <row r="8">
@@ -581,16 +581,16 @@
         <v>26</v>
       </c>
       <c r="B8" t="n">
-        <v>-490031.9999999999</v>
+        <v>-610982</v>
       </c>
       <c r="C8" t="n">
-        <v>-219733.4085850367</v>
+        <v>-405495.5744271266</v>
       </c>
       <c r="D8" t="n">
-        <v>516660.1179171375</v>
+        <v>526172.9897789193</v>
       </c>
       <c r="E8" t="n">
-        <v>-193105.2906678991</v>
+        <v>-490304.5846482073</v>
       </c>
     </row>
     <row r="9">
@@ -598,16 +598,16 @@
         <v>27</v>
       </c>
       <c r="B9" t="n">
-        <v>-456001.9999999999</v>
+        <v>-573727</v>
       </c>
       <c r="C9" t="n">
-        <v>-204040.4627613843</v>
+        <v>-379193.4811358621</v>
       </c>
       <c r="D9" t="n">
-        <v>438724.6058236626</v>
+        <v>447746.5951715267</v>
       </c>
       <c r="E9" t="n">
-        <v>-221317.8569377216</v>
+        <v>-505173.8859643355</v>
       </c>
     </row>
     <row r="10">
@@ -615,16 +615,16 @@
         <v>28</v>
       </c>
       <c r="B10" t="n">
-        <v>-421971.9999999999</v>
+        <v>-536472</v>
       </c>
       <c r="C10" t="n">
-        <v>-188347.5169377318</v>
+        <v>-352891.3878445978</v>
       </c>
       <c r="D10" t="n">
-        <v>367519.3079894771</v>
+        <v>376085.9103500683</v>
       </c>
       <c r="E10" t="n">
-        <v>-242800.2089482547</v>
+        <v>-513277.4774945295</v>
       </c>
     </row>
     <row r="11">
@@ -632,16 +632,16 @@
         <v>29</v>
       </c>
       <c r="B11" t="n">
-        <v>-387941.9999999999</v>
+        <v>-499216.9999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-172654.5711140794</v>
+        <v>-326589.2945533334</v>
       </c>
       <c r="D11" t="n">
-        <v>303564.6604244588</v>
+        <v>311745.7064900743</v>
       </c>
       <c r="E11" t="n">
-        <v>-257031.9106896205</v>
+        <v>-514060.5880632591</v>
       </c>
     </row>
     <row r="12">
@@ -649,16 +649,16 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>-353911.9999999999</v>
+        <v>-461961.9999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>-156961.6252904269</v>
+        <v>-300287.2012620691</v>
       </c>
       <c r="D12" t="n">
-        <v>247088.5132743314</v>
+        <v>254977.6820881198</v>
       </c>
       <c r="E12" t="n">
-        <v>-263785.1120160954</v>
+        <v>-507271.5191739491</v>
       </c>
     </row>
     <row r="13">
@@ -666,16 +666,16 @@
         <v>31</v>
       </c>
       <c r="B13" t="n">
-        <v>-319881.9999999999</v>
+        <v>-424706.9999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>-141268.6794667745</v>
+        <v>-273985.1079708047</v>
       </c>
       <c r="D13" t="n">
-        <v>198033.0673683339</v>
+        <v>205735.2693566457</v>
       </c>
       <c r="E13" t="n">
-        <v>-263117.6120984405</v>
+        <v>-492956.838614159</v>
       </c>
     </row>
     <row r="14">
@@ -683,16 +683,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="n">
-        <v>-285851.9999999999</v>
+        <v>-387451.9999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-125575.7336431221</v>
+        <v>-247683.0146795403</v>
       </c>
       <c r="D14" t="n">
-        <v>156091.9745967096</v>
+        <v>163711.3015638065</v>
       </c>
       <c r="E14" t="n">
-        <v>-255335.7590464124</v>
+        <v>-471423.7131157338</v>
       </c>
     </row>
     <row r="15">
@@ -700,16 +700,16 @@
         <v>33</v>
       </c>
       <c r="B15" t="n">
-        <v>-251821.9999999999</v>
+        <v>-350196.9999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-109882.7878194696</v>
+        <v>-221380.921388276</v>
       </c>
       <c r="D15" t="n">
-        <v>120766.1125026441</v>
+        <v>128396.2561726109</v>
       </c>
       <c r="E15" t="n">
-        <v>-240938.6753168255</v>
+        <v>-443181.665215665</v>
       </c>
     </row>
     <row r="16">
@@ -717,16 +717,16 @@
         <v>34</v>
       </c>
       <c r="B16" t="n">
-        <v>-217791.9999999999</v>
+        <v>-312941.9999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>-94189.84199581717</v>
+        <v>-195078.8280970116</v>
       </c>
       <c r="D16" t="n">
-        <v>91426.40617033467</v>
+        <v>99144.44133079801</v>
       </c>
       <c r="E16" t="n">
-        <v>-220555.4358254825</v>
+        <v>-408876.3867662135</v>
       </c>
     </row>
     <row r="17">
@@ -734,16 +734,16 @@
         <v>35</v>
       </c>
       <c r="B17" t="n">
-        <v>-183761.9999999999</v>
+        <v>-275686.9999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>-78496.89617216476</v>
+        <v>-168776.7348057472</v>
       </c>
       <c r="D17" t="n">
-        <v>67374.24185788355</v>
+        <v>75237.78847215626</v>
       </c>
       <c r="E17" t="n">
-        <v>-194884.6543142812</v>
+        <v>-369225.9463335908</v>
       </c>
     </row>
     <row r="18">
@@ -751,16 +751,16 @@
         <v>36</v>
       </c>
       <c r="B18" t="n">
-        <v>-149731.9999999999</v>
+        <v>-238431.9999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>-62803.95034851233</v>
+        <v>-142474.6415144828</v>
       </c>
       <c r="D18" t="n">
-        <v>47893.2085016945</v>
+        <v>55940.40061255813</v>
       </c>
       <c r="E18" t="n">
-        <v>-164642.7418468178</v>
+        <v>-324966.2409019247</v>
       </c>
     </row>
     <row r="19">
@@ -768,16 +768,16 @@
         <v>37</v>
       </c>
       <c r="B19" t="n">
-        <v>-115702</v>
+        <v>-201176.9999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>-47111.00452485986</v>
+        <v>-116172.5482232185</v>
       </c>
       <c r="D19" t="n">
-        <v>32289.0808886994</v>
+        <v>40540.50302424414</v>
       </c>
       <c r="E19" t="n">
-        <v>-130523.9236361604</v>
+        <v>-276809.0451989743</v>
       </c>
     </row>
     <row r="20">
@@ -785,16 +785,16 @@
         <v>38</v>
       </c>
       <c r="B20" t="n">
-        <v>-81671.99999999996</v>
+        <v>-163921.9999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>-31418.05870120745</v>
+        <v>-89870.4549319541</v>
       </c>
       <c r="D20" t="n">
-        <v>19917.507651767</v>
+        <v>28379.24532884999</v>
       </c>
       <c r="E20" t="n">
-        <v>-93172.5510494404</v>
+        <v>-225413.209603104</v>
       </c>
     </row>
     <row r="21">
@@ -802,16 +802,16 @@
         <v>39</v>
       </c>
       <c r="B21" t="n">
-        <v>-47641.99999999995</v>
+        <v>-126666.9999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>-15725.11287755502</v>
+        <v>-63568.36164068966</v>
       </c>
       <c r="D21" t="n">
-        <v>10200.56481716832</v>
+        <v>18867.65578032986</v>
       </c>
       <c r="E21" t="n">
-        <v>-53166.54806038665</v>
+        <v>-171367.7058603597</v>
       </c>
     </row>
     <row r="22">
@@ -819,16 +819,16 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>-13611.99999999995</v>
+        <v>-89411.99999999994</v>
       </c>
       <c r="C22" t="n">
-        <v>-32.16705390260904</v>
+        <v>-37266.26834942534</v>
       </c>
       <c r="D22" t="n">
-        <v>2634.227576587983</v>
+        <v>11494.00368715843</v>
       </c>
       <c r="E22" t="n">
-        <v>-11009.93947731458</v>
+        <v>-115184.2646622669</v>
       </c>
     </row>
     <row r="23">
@@ -836,16 +836,16 @@
         <v>41</v>
       </c>
       <c r="B23" t="n">
-        <v>20418.00000000005</v>
+        <v>-52156.99999999995</v>
       </c>
       <c r="C23" t="n">
-        <v>15660.77876974983</v>
+        <v>-10964.17505816105</v>
       </c>
       <c r="D23" t="n">
-        <v>-3210.917879820435</v>
+        <v>5824.094069828895</v>
       </c>
       <c r="E23" t="n">
-        <v>32867.86088992943</v>
+        <v>-57297.08098833211</v>
       </c>
     </row>
     <row r="24">
@@ -853,16 +853,16 @@
         <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>54448.00000000005</v>
+        <v>-14901.99999999995</v>
       </c>
       <c r="C24" t="n">
-        <v>31353.72459340224</v>
+        <v>15337.91823310338</v>
       </c>
       <c r="D24" t="n">
-        <v>-7693.536970337405</v>
+        <v>1496.846231199273</v>
       </c>
       <c r="E24" t="n">
-        <v>78108.18762306489</v>
+        <v>1932.764464302706</v>
       </c>
     </row>
     <row r="25">
@@ -870,16 +870,16 @@
         <v>43</v>
       </c>
       <c r="B25" t="n">
-        <v>88478.00000000004</v>
+        <v>22353.00000000005</v>
       </c>
       <c r="C25" t="n">
-        <v>47046.67041705467</v>
+        <v>41640.0115243677</v>
       </c>
       <c r="D25" t="n">
-        <v>-11108.14873614327</v>
+        <v>-1782.89062068315</v>
       </c>
       <c r="E25" t="n">
-        <v>124416.5216809115</v>
+        <v>62210.1209036846</v>
       </c>
     </row>
     <row r="26">
@@ -887,16 +887,16 @@
         <v>44</v>
       </c>
       <c r="B26" t="n">
-        <v>122508</v>
+        <v>59608.00000000005</v>
       </c>
       <c r="C26" t="n">
-        <v>62739.6162407072</v>
+        <v>67942.10481563213</v>
       </c>
       <c r="D26" t="n">
-        <v>-13693.05615244248</v>
+        <v>-4252.80108535308</v>
       </c>
       <c r="E26" t="n">
-        <v>171554.5600882648</v>
+        <v>123297.3037302791</v>
       </c>
     </row>
     <row r="27">
@@ -904,16 +904,16 @@
         <v>45</v>
       </c>
       <c r="B27" t="n">
-        <v>156538.0000000001</v>
+        <v>96863.00000000006</v>
       </c>
       <c r="C27" t="n">
-        <v>78432.5620643596</v>
+        <v>94244.19810689645</v>
       </c>
       <c r="D27" t="n">
-        <v>-15638.60273696359</v>
+        <v>-6101.808381462612</v>
       </c>
       <c r="E27" t="n">
-        <v>219331.9593273961</v>
+        <v>185005.3897254339</v>
       </c>
     </row>
   </sheetData>
@@ -967,16 +967,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-694212</v>
+        <v>-834512</v>
       </c>
       <c r="C2" t="n">
-        <v>-314528.902680247</v>
+        <v>-564110.0985171185</v>
       </c>
       <c r="D2" t="n">
-        <v>1080186.349496508</v>
+        <v>1090112.915852188</v>
       </c>
       <c r="E2" t="n">
-        <v>71445.44681626104</v>
+        <v>-308509.1826649306</v>
       </c>
     </row>
     <row r="3">
@@ -984,16 +984,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-660182</v>
+        <v>-797257</v>
       </c>
       <c r="C3" t="n">
-        <v>-298867.8478142594</v>
+        <v>-537848.1034429744</v>
       </c>
       <c r="D3" t="n">
-        <v>980960.2924452492</v>
+        <v>990886.858800929</v>
       </c>
       <c r="E3" t="n">
-        <v>21910.4446309898</v>
+        <v>-344218.2446420453</v>
       </c>
     </row>
     <row r="4">
@@ -1001,16 +1001,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-626152</v>
+        <v>-760002</v>
       </c>
       <c r="C4" t="n">
-        <v>-283206.7929482717</v>
+        <v>-511586.1083688303</v>
       </c>
       <c r="D4" t="n">
-        <v>882634.4930528447</v>
+        <v>892561.0594085245</v>
       </c>
       <c r="E4" t="n">
-        <v>-26724.29989542696</v>
+        <v>-379027.0489603058</v>
       </c>
     </row>
     <row r="5">
@@ -1018,16 +1018,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-592122</v>
+        <v>-722747</v>
       </c>
       <c r="C5" t="n">
-        <v>-267545.738082284</v>
+        <v>-485324.1132946863</v>
       </c>
       <c r="D5" t="n">
-        <v>785884.8929413116</v>
+        <v>795811.4592969915</v>
       </c>
       <c r="E5" t="n">
-        <v>-73782.84514097252</v>
+        <v>-412259.6539976947</v>
       </c>
     </row>
     <row r="6">
@@ -1035,16 +1035,16 @@
         <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>-558092</v>
+        <v>-685492</v>
       </c>
       <c r="C6" t="n">
-        <v>-251884.6832162964</v>
+        <v>-459062.1182205422</v>
       </c>
       <c r="D6" t="n">
-        <v>691625.0230690287</v>
+        <v>701551.5894247086</v>
       </c>
       <c r="E6" t="n">
-        <v>-118351.6601472676</v>
+        <v>-443002.5287958335</v>
       </c>
     </row>
     <row r="7">
@@ -1052,16 +1052,16 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>-524061.9999999999</v>
+        <v>-648237</v>
       </c>
       <c r="C7" t="n">
-        <v>-236223.6283503087</v>
+        <v>-432800.1231463981</v>
       </c>
       <c r="D7" t="n">
-        <v>600955.2296958403</v>
+        <v>610881.7960515202</v>
       </c>
       <c r="E7" t="n">
-        <v>-159330.3986544684</v>
+        <v>-470155.3270948778</v>
       </c>
     </row>
     <row r="8">
@@ -1069,16 +1069,16 @@
         <v>26</v>
       </c>
       <c r="B8" t="n">
-        <v>-490031.9999999999</v>
+        <v>-610982</v>
       </c>
       <c r="C8" t="n">
-        <v>-220562.5734843211</v>
+        <v>-406538.1280722541</v>
       </c>
       <c r="D8" t="n">
-        <v>515060.3157666151</v>
+        <v>524986.882122295</v>
       </c>
       <c r="E8" t="n">
-        <v>-195534.2577177059</v>
+        <v>-492533.2459499591</v>
       </c>
     </row>
     <row r="9">
@@ -1086,16 +1086,16 @@
         <v>27</v>
       </c>
       <c r="B9" t="n">
-        <v>-456001.9999999999</v>
+        <v>-573727</v>
       </c>
       <c r="C9" t="n">
-        <v>-204901.5186183334</v>
+        <v>-380276.1329981099</v>
       </c>
       <c r="D9" t="n">
-        <v>435076.8668778502</v>
+        <v>445003.43323353</v>
       </c>
       <c r="E9" t="n">
-        <v>-225826.6517404832</v>
+        <v>-508999.6997645799</v>
       </c>
     </row>
     <row r="10">
@@ -1103,16 +1103,16 @@
         <v>28</v>
       </c>
       <c r="B10" t="n">
-        <v>-421971.9999999999</v>
+        <v>-536472</v>
       </c>
       <c r="C10" t="n">
-        <v>-189240.4637523457</v>
+        <v>-354014.1379239658</v>
       </c>
       <c r="D10" t="n">
-        <v>361961.1220410502</v>
+        <v>371887.6883967301</v>
       </c>
       <c r="E10" t="n">
-        <v>-249251.3417112955</v>
+        <v>-518598.4495272358</v>
       </c>
     </row>
     <row r="11">
@@ -1120,16 +1120,16 @@
         <v>29</v>
       </c>
       <c r="B11" t="n">
-        <v>-387941.9999999999</v>
+        <v>-499216.9999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-173579.4088863581</v>
+        <v>-327752.1428498218</v>
       </c>
       <c r="D11" t="n">
-        <v>296386.332122053</v>
+        <v>306312.8984777328</v>
       </c>
       <c r="E11" t="n">
-        <v>-265135.0767643051</v>
+        <v>-520656.2443720889</v>
       </c>
     </row>
     <row r="12">
@@ -1137,16 +1137,16 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>-353911.9999999999</v>
+        <v>-461961.9999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>-157918.3540203705</v>
+        <v>-301490.1477756777</v>
       </c>
       <c r="D12" t="n">
-        <v>238687.6287908625</v>
+        <v>248614.1951465424</v>
       </c>
       <c r="E12" t="n">
-        <v>-273142.7252295079</v>
+        <v>-514837.9526291353</v>
       </c>
     </row>
     <row r="13">
@@ -1154,16 +1154,16 @@
         <v>31</v>
       </c>
       <c r="B13" t="n">
-        <v>-319881.9999999999</v>
+        <v>-424706.9999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>-142257.2991543828</v>
+        <v>-275228.1527015336</v>
       </c>
       <c r="D13" t="n">
-        <v>188858.18852895</v>
+        <v>198784.7548846299</v>
       </c>
       <c r="E13" t="n">
-        <v>-273281.1106254327</v>
+        <v>-501150.3978169037</v>
       </c>
     </row>
     <row r="14">
@@ -1171,16 +1171,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="n">
-        <v>-285851.9999999999</v>
+        <v>-387451.9999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-126596.2442883952</v>
+        <v>-248966.1576273896</v>
       </c>
       <c r="D14" t="n">
-        <v>146588.3881771265</v>
+        <v>156514.9545328064</v>
       </c>
       <c r="E14" t="n">
-        <v>-265859.8561112686</v>
+        <v>-479903.2030945831</v>
       </c>
     </row>
     <row r="15">
@@ -1188,16 +1188,16 @@
         <v>33</v>
       </c>
       <c r="B15" t="n">
-        <v>-251821.9999999999</v>
+        <v>-350196.9999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-110935.1894224075</v>
+        <v>-222704.1625532456</v>
       </c>
       <c r="D15" t="n">
-        <v>111332.7860138555</v>
+        <v>121259.3523695355</v>
       </c>
       <c r="E15" t="n">
-        <v>-251424.4034085519</v>
+        <v>-451641.81018371</v>
       </c>
     </row>
     <row r="16">
@@ -1205,16 +1205,16 @@
         <v>34</v>
       </c>
       <c r="B16" t="n">
-        <v>-217791.9999999999</v>
+        <v>-312941.9999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>-95274.1345564198</v>
+        <v>-196442.1674791013</v>
       </c>
       <c r="D16" t="n">
-        <v>82388.45564648526</v>
+        <v>92315.02200216516</v>
       </c>
       <c r="E16" t="n">
-        <v>-230677.6789099345</v>
+        <v>-417069.1454769361</v>
       </c>
     </row>
     <row r="17">
@@ -1222,16 +1222,16 @@
         <v>35</v>
       </c>
       <c r="B17" t="n">
-        <v>-183761.9999999999</v>
+        <v>-275686.9999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>-79613.07969043223</v>
+        <v>-170180.1724049574</v>
       </c>
       <c r="D17" t="n">
-        <v>58970.93530230709</v>
+        <v>68897.50165798698</v>
       </c>
       <c r="E17" t="n">
-        <v>-204404.1443881251</v>
+        <v>-376969.6707469703</v>
       </c>
     </row>
     <row r="18">
@@ -1239,16 +1239,16 @@
         <v>36</v>
       </c>
       <c r="B18" t="n">
-        <v>-149731.9999999999</v>
+        <v>-238431.9999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>-63952.02482444455</v>
+        <v>-143918.1773308133</v>
       </c>
       <c r="D18" t="n">
-        <v>40278.71029007911</v>
+        <v>50205.276645759</v>
       </c>
       <c r="E18" t="n">
-        <v>-173405.3145343654</v>
+        <v>-332144.9006850543</v>
       </c>
     </row>
     <row r="19">
@@ -1256,16 +1256,16 @@
         <v>37</v>
       </c>
       <c r="B19" t="n">
-        <v>-115702</v>
+        <v>-201176.9999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>-48290.96995845687</v>
+        <v>-117656.1822566692</v>
       </c>
       <c r="D19" t="n">
-        <v>25541.91376984261</v>
+        <v>35468.48012552252</v>
       </c>
       <c r="E19" t="n">
-        <v>-138451.0561886142</v>
+        <v>-283364.7021311466</v>
       </c>
     </row>
     <row r="20">
@@ -1273,16 +1273,16 @@
         <v>38</v>
       </c>
       <c r="B20" t="n">
-        <v>-81671.99999999996</v>
+        <v>-163921.9999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>-32629.91509246922</v>
+        <v>-91394.18718252509</v>
       </c>
       <c r="D20" t="n">
-        <v>14054.72060008546</v>
+        <v>23981.28695576537</v>
       </c>
       <c r="E20" t="n">
-        <v>-100247.1944923837</v>
+        <v>-231334.9002267597</v>
       </c>
     </row>
     <row r="21">
@@ -1290,16 +1290,16 @@
         <v>39</v>
       </c>
       <c r="B21" t="n">
-        <v>-47641.99999999995</v>
+        <v>-126666.9999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>-16968.86022648157</v>
+        <v>-65132.19210838102</v>
       </c>
       <c r="D21" t="n">
-        <v>5193.33554477745</v>
+        <v>15119.90190045736</v>
       </c>
       <c r="E21" t="n">
-        <v>-59417.52468170407</v>
+        <v>-176679.2902079236</v>
       </c>
     </row>
     <row r="22">
@@ -1307,16 +1307,16 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>-13611.99999999995</v>
+        <v>-89411.99999999994</v>
       </c>
       <c r="C22" t="n">
-        <v>-1307.805360494007</v>
+        <v>-38870.19703423709</v>
       </c>
       <c r="D22" t="n">
-        <v>-1577.361134174926</v>
+        <v>8349.205221504979</v>
       </c>
       <c r="E22" t="n">
-        <v>-16497.16649466888</v>
+        <v>-119932.9918127321</v>
       </c>
     </row>
     <row r="23">
@@ -1324,16 +1324,16 @@
         <v>41</v>
       </c>
       <c r="B23" t="n">
-        <v>20418.00000000005</v>
+        <v>-52156.99999999995</v>
       </c>
       <c r="C23" t="n">
-        <v>14353.2495054937</v>
+        <v>-12608.20196009291</v>
       </c>
       <c r="D23" t="n">
-        <v>-6705.221143104828</v>
+        <v>3221.345212575077</v>
       </c>
       <c r="E23" t="n">
-        <v>28066.02836238892</v>
+        <v>-61543.85674751778</v>
       </c>
     </row>
     <row r="24">
@@ -1341,16 +1341,16 @@
         <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>54448.00000000005</v>
+        <v>-14901.99999999995</v>
       </c>
       <c r="C24" t="n">
-        <v>30014.30437148135</v>
+        <v>13653.79311405116</v>
       </c>
       <c r="D24" t="n">
-        <v>-10557.33718220033</v>
+        <v>-630.7708265204215</v>
       </c>
       <c r="E24" t="n">
-        <v>73904.96718928109</v>
+        <v>-1878.977712469204</v>
       </c>
     </row>
     <row r="25">
@@ -1358,16 +1358,16 @@
         <v>43</v>
       </c>
       <c r="B25" t="n">
-        <v>88478.00000000004</v>
+        <v>22353.00000000005</v>
       </c>
       <c r="C25" t="n">
-        <v>45675.35923746901</v>
+        <v>39915.78818819523</v>
       </c>
       <c r="D25" t="n">
-        <v>-13429.29748422697</v>
+        <v>-3502.731128547068</v>
       </c>
       <c r="E25" t="n">
-        <v>120724.0617532421</v>
+        <v>58766.05705964823</v>
       </c>
     </row>
     <row r="26">
@@ -1375,16 +1375,16 @@
         <v>44</v>
       </c>
       <c r="B26" t="n">
-        <v>122508</v>
+        <v>59608.00000000005</v>
       </c>
       <c r="C26" t="n">
-        <v>61336.41410345669</v>
+        <v>66177.78326233939</v>
       </c>
       <c r="D26" t="n">
-        <v>-15555.47390223187</v>
+        <v>-5628.907546551963</v>
       </c>
       <c r="E26" t="n">
-        <v>168288.9402012248</v>
+        <v>120156.8757157875</v>
       </c>
     </row>
     <row r="27">
@@ -1392,16 +1392,16 @@
         <v>45</v>
       </c>
       <c r="B27" t="n">
-        <v>156538.0000000001</v>
+        <v>96863.00000000006</v>
       </c>
       <c r="C27" t="n">
-        <v>76997.46896944431</v>
+        <v>92439.77833648337</v>
       </c>
       <c r="D27" t="n">
-        <v>-17119.20741477291</v>
+        <v>-7192.641059093</v>
       </c>
       <c r="E27" t="n">
-        <v>216416.2615546715</v>
+        <v>182110.1372773904</v>
       </c>
     </row>
   </sheetData>
@@ -1455,16 +1455,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-694212</v>
+        <v>-834512</v>
       </c>
       <c r="C2" t="n">
-        <v>-316988.2330259276</v>
+        <v>-568234.1452034132</v>
       </c>
       <c r="D2" t="n">
-        <v>1104837.027287472</v>
+        <v>1114763.593643152</v>
       </c>
       <c r="E2" t="n">
-        <v>93636.79426154448</v>
+        <v>-287982.5515602615</v>
       </c>
     </row>
     <row r="3">
@@ -1472,16 +1472,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-660182</v>
+        <v>-797257</v>
       </c>
       <c r="C3" t="n">
-        <v>-301450.1446772239</v>
+        <v>-542178.3524635838</v>
       </c>
       <c r="D3" t="n">
-        <v>1004850.320950248</v>
+        <v>1014776.887305928</v>
       </c>
       <c r="E3" t="n">
-        <v>43218.17627302452</v>
+        <v>-324658.4651576556</v>
       </c>
     </row>
     <row r="4">
@@ -1489,16 +1489,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-626152</v>
+        <v>-760002</v>
       </c>
       <c r="C4" t="n">
-        <v>-285912.0563285203</v>
+        <v>-516122.5597237545</v>
       </c>
       <c r="D4" t="n">
-        <v>904910.0109337254</v>
+        <v>914836.5772894053</v>
       </c>
       <c r="E4" t="n">
-        <v>-7154.045394794899</v>
+        <v>-361287.9824343491</v>
       </c>
     </row>
     <row r="5">
@@ -1506,16 +1506,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-592122</v>
+        <v>-722747</v>
       </c>
       <c r="C5" t="n">
-        <v>-270373.9679798166</v>
+        <v>-490066.7669839251</v>
       </c>
       <c r="D5" t="n">
-        <v>805136.0236275727</v>
+        <v>815062.5899832526</v>
       </c>
       <c r="E5" t="n">
-        <v>-57359.94435224391</v>
+        <v>-397751.1770006726</v>
       </c>
     </row>
     <row r="6">
@@ -1523,16 +1523,16 @@
         <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>-558092</v>
+        <v>-685492</v>
       </c>
       <c r="C6" t="n">
-        <v>-254835.879631113</v>
+        <v>-464010.9742440957</v>
       </c>
       <c r="D6" t="n">
-        <v>705857.2899582346</v>
+        <v>715783.8563139145</v>
       </c>
       <c r="E6" t="n">
-        <v>-107070.5896728784</v>
+        <v>-433719.1179301813</v>
       </c>
     </row>
     <row r="7">
@@ -1540,16 +1540,16 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>-524061.9999999999</v>
+        <v>-648237</v>
       </c>
       <c r="C7" t="n">
-        <v>-239297.7912824094</v>
+        <v>-437955.1815042665</v>
       </c>
       <c r="D7" t="n">
-        <v>607805.1181869153</v>
+        <v>617731.6845425952</v>
       </c>
       <c r="E7" t="n">
-        <v>-155554.673095494</v>
+        <v>-468460.4969616712</v>
       </c>
     </row>
     <row r="8">
@@ -1557,16 +1557,16 @@
         <v>26</v>
       </c>
       <c r="B8" t="n">
-        <v>-490031.9999999999</v>
+        <v>-610982</v>
       </c>
       <c r="C8" t="n">
-        <v>-223759.7029337058</v>
+        <v>-411899.3887644371</v>
       </c>
       <c r="D8" t="n">
-        <v>512298.7767659657</v>
+        <v>522225.3431216456</v>
       </c>
       <c r="E8" t="n">
-        <v>-201492.9261677399</v>
+        <v>-500656.0456427914</v>
       </c>
     </row>
     <row r="9">
@@ -1574,16 +1574,16 @@
         <v>27</v>
       </c>
       <c r="B9" t="n">
-        <v>-456001.9999999999</v>
+        <v>-573727</v>
       </c>
       <c r="C9" t="n">
-        <v>-208221.6145850021</v>
+        <v>-385843.5960246078</v>
       </c>
       <c r="D9" t="n">
-        <v>421273.2641746689</v>
+        <v>431199.8305303488</v>
       </c>
       <c r="E9" t="n">
-        <v>-242950.3504103332</v>
+        <v>-528370.7654942591</v>
       </c>
     </row>
     <row r="10">
@@ -1591,16 +1591,16 @@
         <v>28</v>
       </c>
       <c r="B10" t="n">
-        <v>-421971.9999999999</v>
+        <v>-536472</v>
       </c>
       <c r="C10" t="n">
-        <v>-192683.5262362985</v>
+        <v>-359787.8032847784</v>
       </c>
       <c r="D10" t="n">
-        <v>337029.7963381566</v>
+        <v>346956.3626938364</v>
       </c>
       <c r="E10" t="n">
-        <v>-277625.7298981418</v>
+        <v>-549303.4405909419</v>
       </c>
     </row>
     <row r="11">
@@ -1608,16 +1608,16 @@
         <v>29</v>
       </c>
       <c r="B11" t="n">
-        <v>-387941.9999999999</v>
+        <v>-499216.9999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-177145.4378875949</v>
+        <v>-333732.0105449492</v>
       </c>
       <c r="D11" t="n">
-        <v>261747.5728784995</v>
+        <v>271674.1392341793</v>
       </c>
       <c r="E11" t="n">
-        <v>-303339.8650090953</v>
+        <v>-561274.8713107698</v>
       </c>
     </row>
     <row r="12">
@@ -1625,16 +1625,16 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>-353911.9999999999</v>
+        <v>-461961.9999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>-161607.3495388913</v>
+        <v>-307676.2178051197</v>
       </c>
       <c r="D12" t="n">
-        <v>196963.2031256775</v>
+        <v>206889.7694813574</v>
       </c>
       <c r="E12" t="n">
-        <v>-318556.1464132137</v>
+        <v>-562748.4483237623</v>
       </c>
     </row>
     <row r="13">
@@ -1642,16 +1642,16 @@
         <v>31</v>
       </c>
       <c r="B13" t="n">
-        <v>-319881.9999999999</v>
+        <v>-424706.9999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>-146069.2611901876</v>
+        <v>-281620.4250652904</v>
       </c>
       <c r="D13" t="n">
-        <v>143254.1901844384</v>
+        <v>153180.7565401183</v>
       </c>
       <c r="E13" t="n">
-        <v>-322697.0710057491</v>
+        <v>-553146.6685251722</v>
       </c>
     </row>
     <row r="14">
@@ -1659,16 +1659,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="n">
-        <v>-285851.9999999999</v>
+        <v>-387451.9999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-130531.172841484</v>
+        <v>-255564.6323254611</v>
       </c>
       <c r="D14" t="n">
-        <v>100234.8907216942</v>
+        <v>110161.4570773741</v>
       </c>
       <c r="E14" t="n">
-        <v>-316148.2821197898</v>
+        <v>-532855.1752480869</v>
       </c>
     </row>
     <row r="15">
@@ -1676,16 +1676,16 @@
         <v>33</v>
       </c>
       <c r="B15" t="n">
-        <v>-251821.9999999999</v>
+        <v>-350196.9999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-114993.0844927804</v>
+        <v>-229508.8395856316</v>
       </c>
       <c r="D15" t="n">
-        <v>66802.53065266434</v>
+        <v>76729.09700834424</v>
       </c>
       <c r="E15" t="n">
-        <v>-300012.5538401159</v>
+        <v>-502976.7425772874</v>
       </c>
     </row>
     <row r="16">
@@ -1693,16 +1693,16 @@
         <v>34</v>
       </c>
       <c r="B16" t="n">
-        <v>-217791.9999999999</v>
+        <v>-312941.9999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>-99454.99614407675</v>
+        <v>-203453.0468458023</v>
       </c>
       <c r="D16" t="n">
-        <v>41479.24734720539</v>
+        <v>51405.81370288529</v>
       </c>
       <c r="E16" t="n">
-        <v>-275767.7487968713</v>
+        <v>-464989.233142917</v>
       </c>
     </row>
     <row r="17">
@@ -1710,16 +1710,16 @@
         <v>35</v>
       </c>
       <c r="B17" t="n">
-        <v>-183761.9999999999</v>
+        <v>-275686.9999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>-83916.90779537318</v>
+        <v>-177397.2541059731</v>
       </c>
       <c r="D17" t="n">
-        <v>22712.64131547301</v>
+        <v>32639.20767115292</v>
       </c>
       <c r="E17" t="n">
-        <v>-244966.2664799001</v>
+        <v>-420445.0464348202</v>
       </c>
     </row>
     <row r="18">
@@ -1727,16 +1727,16 @@
         <v>36</v>
       </c>
       <c r="B18" t="n">
-        <v>-149731.9999999999</v>
+        <v>-238431.9999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>-68378.81944666951</v>
+        <v>-151341.4613661437</v>
       </c>
       <c r="D18" t="n">
-        <v>9070.16917260222</v>
+        <v>18996.73552828213</v>
       </c>
       <c r="E18" t="n">
-        <v>-209040.6502740672</v>
+        <v>-370776.7258378615</v>
       </c>
     </row>
     <row r="19">
@@ -1744,16 +1744,16 @@
         <v>37</v>
       </c>
       <c r="B19" t="n">
-        <v>-115702</v>
+        <v>-201176.9999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>-52840.73109796591</v>
+        <v>-125285.6686263144</v>
       </c>
       <c r="D19" t="n">
-        <v>-670.8543224704933</v>
+        <v>9255.712033209413</v>
       </c>
       <c r="E19" t="n">
-        <v>-169213.5854204363</v>
+        <v>-317206.9565931049</v>
       </c>
     </row>
     <row r="20">
@@ -1761,16 +1761,16 @@
         <v>38</v>
       </c>
       <c r="B20" t="n">
-        <v>-81671.99999999996</v>
+        <v>-163921.9999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>-37302.64274926222</v>
+        <v>-99229.87588648492</v>
       </c>
       <c r="D20" t="n">
-        <v>-7504.362366704179</v>
+        <v>2422.203988975725</v>
       </c>
       <c r="E20" t="n">
-        <v>-126479.0051159664</v>
+        <v>-260729.6718975091</v>
       </c>
     </row>
     <row r="21">
@@ -1778,16 +1778,16 @@
         <v>39</v>
       </c>
       <c r="B21" t="n">
-        <v>-47641.99999999995</v>
+        <v>-126666.9999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>-21764.55440055867</v>
+        <v>-73174.08314665573</v>
       </c>
       <c r="D21" t="n">
-        <v>-12212.95013673058</v>
+        <v>-2286.383781050673</v>
       </c>
       <c r="E21" t="n">
-        <v>-81619.50453728919</v>
+        <v>-202127.4669277064</v>
       </c>
     </row>
     <row r="22">
@@ -1795,16 +1795,16 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>-13611.99999999995</v>
+        <v>-89411.99999999994</v>
       </c>
       <c r="C22" t="n">
-        <v>-6226.466051855066</v>
+        <v>-47118.29040682642</v>
       </c>
       <c r="D22" t="n">
-        <v>-15398.34766175634</v>
+        <v>-5471.781306076428</v>
       </c>
       <c r="E22" t="n">
-        <v>-35236.81371361135</v>
+        <v>-142002.0717129028</v>
       </c>
     </row>
     <row r="23">
@@ -1812,16 +1812,16 @@
         <v>41</v>
       </c>
       <c r="B23" t="n">
-        <v>20418.00000000005</v>
+        <v>-52156.99999999995</v>
       </c>
       <c r="C23" t="n">
-        <v>9311.622296848596</v>
+        <v>-21062.49766699699</v>
       </c>
       <c r="D23" t="n">
-        <v>-17513.49380396767</v>
+        <v>-7586.927448287766</v>
       </c>
       <c r="E23" t="n">
-        <v>12216.12849288097</v>
+        <v>-80806.4251152847</v>
       </c>
     </row>
     <row r="24">
@@ -1829,16 +1829,16 @@
         <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>54448.00000000005</v>
+        <v>-14901.99999999995</v>
       </c>
       <c r="C24" t="n">
-        <v>24849.7106455522</v>
+        <v>4993.295072832319</v>
       </c>
       <c r="D24" t="n">
-        <v>-18892.02059346736</v>
+        <v>-8965.45423778746</v>
       </c>
       <c r="E24" t="n">
-        <v>60405.69005208489</v>
+        <v>-18874.15916495509</v>
       </c>
     </row>
     <row r="25">
@@ -1846,16 +1846,16 @@
         <v>43</v>
       </c>
       <c r="B25" t="n">
-        <v>88478.00000000004</v>
+        <v>22353.00000000005</v>
       </c>
       <c r="C25" t="n">
-        <v>40387.79899425592</v>
+        <v>31049.0878126618</v>
       </c>
       <c r="D25" t="n">
-        <v>-19774.10030548955</v>
+        <v>-9847.533949809642</v>
       </c>
       <c r="E25" t="n">
-        <v>109091.6986887664</v>
+        <v>43554.55386285222</v>
       </c>
     </row>
     <row r="26">
@@ -1863,16 +1863,16 @@
         <v>44</v>
       </c>
       <c r="B26" t="n">
-        <v>122508</v>
+        <v>59608.00000000005</v>
       </c>
       <c r="C26" t="n">
-        <v>55925.88734295947</v>
+        <v>57104.880552491</v>
       </c>
       <c r="D26" t="n">
-        <v>-20328.52851197825</v>
+        <v>-10401.96215629835</v>
       </c>
       <c r="E26" t="n">
-        <v>158105.3588309813</v>
+        <v>106310.9183961927</v>
       </c>
     </row>
     <row r="27">
@@ -1880,16 +1880,16 @@
         <v>45</v>
       </c>
       <c r="B27" t="n">
-        <v>156538.0000000001</v>
+        <v>96863.00000000006</v>
       </c>
       <c r="C27" t="n">
-        <v>71463.97569166313</v>
+        <v>83160.67329232043</v>
       </c>
       <c r="D27" t="n">
-        <v>-20671.08639628213</v>
+        <v>-10744.52004060223</v>
       </c>
       <c r="E27" t="n">
-        <v>207330.8892953811</v>
+        <v>169279.1532517183</v>
       </c>
     </row>
   </sheetData>
@@ -1943,16 +1943,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-694212</v>
+        <v>-834512</v>
       </c>
       <c r="C2" t="n">
-        <v>-318092.5597239187</v>
+        <v>-570085.9886808201</v>
       </c>
       <c r="D2" t="n">
-        <v>1116245.54996352</v>
+        <v>1126172.1163192</v>
       </c>
       <c r="E2" t="n">
-        <v>103940.9902396009</v>
+        <v>-278425.8723616204</v>
       </c>
     </row>
     <row r="3">
@@ -1960,16 +1960,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-660182</v>
+        <v>-797257</v>
       </c>
       <c r="C3" t="n">
-        <v>-302609.6877101147</v>
+        <v>-544122.7881148611</v>
       </c>
       <c r="D3" t="n">
-        <v>1016245.681336357</v>
+        <v>1026172.247692037</v>
       </c>
       <c r="E3" t="n">
-        <v>53453.99362624227</v>
+        <v>-315207.5404228242</v>
       </c>
     </row>
     <row r="4">
@@ -1977,16 +1977,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-626152</v>
+        <v>-760002</v>
       </c>
       <c r="C4" t="n">
-        <v>-287126.8156963106</v>
+        <v>-518159.5875489021</v>
       </c>
       <c r="D4" t="n">
-        <v>916246.7556816097</v>
+        <v>926173.3220372896</v>
       </c>
       <c r="E4" t="n">
-        <v>2967.939985299134</v>
+        <v>-351988.2655116124</v>
       </c>
     </row>
     <row r="5">
@@ -1994,16 +1994,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-592122</v>
+        <v>-722747</v>
       </c>
       <c r="C5" t="n">
-        <v>-271643.9436825066</v>
+        <v>-492196.3869829431</v>
       </c>
       <c r="D5" t="n">
-        <v>816253.3847891089</v>
+        <v>826179.9511447888</v>
       </c>
       <c r="E5" t="n">
-        <v>-47512.55889339768</v>
+        <v>-388763.4358381544</v>
       </c>
     </row>
     <row r="6">
@@ -2011,16 +2011,16 @@
         <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>-558092</v>
+        <v>-685492</v>
       </c>
       <c r="C6" t="n">
-        <v>-256161.0716687025</v>
+        <v>-466233.1864169841</v>
       </c>
       <c r="D6" t="n">
-        <v>716285.6815814341</v>
+        <v>726212.247937114</v>
       </c>
       <c r="E6" t="n">
-        <v>-97967.39008726832</v>
+        <v>-425512.9384798701</v>
       </c>
     </row>
     <row r="7">
@@ -2028,16 +2028,16 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>-524061.9999999999</v>
+        <v>-648237</v>
       </c>
       <c r="C7" t="n">
-        <v>-240678.1996548984</v>
+        <v>-440269.9858510252</v>
       </c>
       <c r="D7" t="n">
-        <v>616419.175400461</v>
+        <v>626345.7417561408</v>
       </c>
       <c r="E7" t="n">
-        <v>-148321.0242544374</v>
+        <v>-462161.2440948844</v>
       </c>
     </row>
     <row r="8">
@@ -2045,16 +2045,16 @@
         <v>26</v>
       </c>
       <c r="B8" t="n">
-        <v>-490031.9999999999</v>
+        <v>-610982</v>
       </c>
       <c r="C8" t="n">
-        <v>-225195.3276410943</v>
+        <v>-414306.7852850661</v>
       </c>
       <c r="D8" t="n">
-        <v>516931.934480852</v>
+        <v>526858.5008365319</v>
       </c>
       <c r="E8" t="n">
-        <v>-198295.3931602424</v>
+        <v>-498430.2844485343</v>
       </c>
     </row>
     <row r="9">
@@ -2062,16 +2062,16 @@
         <v>27</v>
       </c>
       <c r="B9" t="n">
-        <v>-456001.9999999999</v>
+        <v>-573727</v>
       </c>
       <c r="C9" t="n">
-        <v>-209712.4556272903</v>
+        <v>-388343.5847191071</v>
       </c>
       <c r="D9" t="n">
-        <v>418791.3445859333</v>
+        <v>428717.9109416131</v>
       </c>
       <c r="E9" t="n">
-        <v>-246923.111041357</v>
+        <v>-533352.673777494</v>
       </c>
     </row>
     <row r="10">
@@ -2079,16 +2079,16 @@
         <v>28</v>
       </c>
       <c r="B10" t="n">
-        <v>-421971.9999999999</v>
+        <v>-536472</v>
       </c>
       <c r="C10" t="n">
-        <v>-194229.5836134862</v>
+        <v>-362380.3841531481</v>
       </c>
       <c r="D10" t="n">
-        <v>324612.8327549468</v>
+        <v>334539.3991106267</v>
       </c>
       <c r="E10" t="n">
-        <v>-291588.7508585394</v>
+        <v>-564312.9850425215</v>
       </c>
     </row>
     <row r="11">
@@ -2096,16 +2096,16 @@
         <v>29</v>
       </c>
       <c r="B11" t="n">
-        <v>-387941.9999999999</v>
+        <v>-499216.9999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-178746.7115996822</v>
+        <v>-336417.1835871892</v>
       </c>
       <c r="D11" t="n">
-        <v>239122.4404119371</v>
+        <v>249049.006767617</v>
       </c>
       <c r="E11" t="n">
-        <v>-327566.271187745</v>
+        <v>-586585.1768195721</v>
       </c>
     </row>
     <row r="12">
@@ -2113,16 +2113,16 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>-353911.9999999999</v>
+        <v>-461961.9999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>-163263.8395858781</v>
+        <v>-310453.9830212301</v>
       </c>
       <c r="D12" t="n">
-        <v>167427.2548833443</v>
+        <v>177353.8212390243</v>
       </c>
       <c r="E12" t="n">
-        <v>-349748.5847025337</v>
+        <v>-595062.1617822057</v>
       </c>
     </row>
     <row r="13">
@@ -2130,16 +2130,16 @@
         <v>31</v>
       </c>
       <c r="B13" t="n">
-        <v>-319881.9999999999</v>
+        <v>-424706.9999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>-147780.9675720741</v>
+        <v>-284490.7824552712</v>
       </c>
       <c r="D13" t="n">
-        <v>111913.1058266379</v>
+        <v>121839.6721823178</v>
       </c>
       <c r="E13" t="n">
-        <v>-355749.8617454361</v>
+        <v>-587358.1102729533</v>
       </c>
     </row>
     <row r="14">
@@ -2147,16 +2147,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="n">
-        <v>-285851.9999999999</v>
+        <v>-387451.9999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-132298.09555827</v>
+        <v>-258527.5818893122</v>
       </c>
       <c r="D14" t="n">
-        <v>71170.31435434676</v>
+        <v>81096.88071002666</v>
       </c>
       <c r="E14" t="n">
-        <v>-346979.7812039232</v>
+        <v>-564882.7011792855</v>
       </c>
     </row>
     <row r="15">
@@ -2164,16 +2164,16 @@
         <v>33</v>
       </c>
       <c r="B15" t="n">
-        <v>-251821.9999999999</v>
+        <v>-350196.9999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-116815.2235444659</v>
+        <v>-232564.3813233532</v>
       </c>
       <c r="D15" t="n">
-        <v>41841.72717672242</v>
+        <v>51768.29353240233</v>
       </c>
       <c r="E15" t="n">
-        <v>-326795.4963677434</v>
+        <v>-530993.0877909508</v>
       </c>
     </row>
     <row r="16">
@@ -2181,16 +2181,16 @@
         <v>34</v>
       </c>
       <c r="B16" t="n">
-        <v>-217791.9999999999</v>
+        <v>-312941.9999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>-101332.3515306619</v>
+        <v>-206601.1807573943</v>
       </c>
       <c r="D16" t="n">
-        <v>20811.21950757959</v>
+        <v>30737.7858632595</v>
       </c>
       <c r="E16" t="n">
-        <v>-298313.1320230822</v>
+        <v>-488805.3948941347</v>
       </c>
     </row>
     <row r="17">
@@ -2198,16 +2198,16 @@
         <v>35</v>
       </c>
       <c r="B17" t="n">
-        <v>-183761.9999999999</v>
+        <v>-275686.9999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>-85849.47951685777</v>
+        <v>-180637.9801914351</v>
       </c>
       <c r="D17" t="n">
-        <v>5919.32831518167</v>
+        <v>15845.89467086157</v>
       </c>
       <c r="E17" t="n">
-        <v>-263692.1512016761</v>
+        <v>-440479.0855205735</v>
       </c>
     </row>
     <row r="18">
@@ -2215,16 +2215,16 @@
         <v>36</v>
       </c>
       <c r="B18" t="n">
-        <v>-149731.9999999999</v>
+        <v>-238431.9999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>-70366.60750305373</v>
+        <v>-154674.7796254762</v>
       </c>
       <c r="D18" t="n">
-        <v>-4323.47445588131</v>
+        <v>5603.091899798595</v>
       </c>
       <c r="E18" t="n">
-        <v>-224422.081958935</v>
+        <v>-387503.6877256776</v>
       </c>
     </row>
     <row r="19">
@@ -2232,16 +2232,16 @@
         <v>37</v>
       </c>
       <c r="B19" t="n">
-        <v>-115702</v>
+        <v>-201176.9999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>-54883.73548924967</v>
+        <v>-128711.5790595172</v>
       </c>
       <c r="D19" t="n">
-        <v>-11090.61559105184</v>
+        <v>-1164.049235371933</v>
       </c>
       <c r="E19" t="n">
-        <v>-181676.3510803015</v>
+        <v>-331052.6282948891</v>
       </c>
     </row>
     <row r="20">
@@ -2249,16 +2249,16 @@
         <v>38</v>
       </c>
       <c r="B20" t="n">
-        <v>-81671.99999999996</v>
+        <v>-163921.9999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>-39400.86347544563</v>
+        <v>-102748.3784935582</v>
       </c>
       <c r="D20" t="n">
-        <v>-15367.22207317064</v>
+        <v>-5440.655717490738</v>
       </c>
       <c r="E20" t="n">
-        <v>-136440.0855486162</v>
+        <v>-272111.0342110489</v>
       </c>
     </row>
     <row r="21">
@@ -2266,16 +2266,16 @@
         <v>39</v>
       </c>
       <c r="B21" t="n">
-        <v>-47641.99999999995</v>
+        <v>-126666.9999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>-23917.99146164153</v>
+        <v>-76785.1779275992</v>
       </c>
       <c r="D21" t="n">
-        <v>-17952.34850604305</v>
+        <v>-8025.782150363139</v>
       </c>
       <c r="E21" t="n">
-        <v>-89512.33996768453</v>
+        <v>-211477.9600779623</v>
       </c>
     </row>
     <row r="22">
@@ -2283,16 +2283,16 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>-13611.99999999995</v>
+        <v>-89411.99999999994</v>
       </c>
       <c r="C22" t="n">
-        <v>-8435.119447837467</v>
+        <v>-50821.97736164019</v>
       </c>
       <c r="D22" t="n">
-        <v>-19449.54996864095</v>
+        <v>-9522.983612961043</v>
       </c>
       <c r="E22" t="n">
-        <v>-41496.66941647837</v>
+        <v>-149756.9609746012</v>
       </c>
     </row>
     <row r="23">
@@ -2300,16 +2300,16 @@
         <v>41</v>
       </c>
       <c r="B23" t="n">
-        <v>20418.00000000005</v>
+        <v>-52156.99999999995</v>
       </c>
       <c r="C23" t="n">
-        <v>7047.752565966599</v>
+        <v>-24858.77679568119</v>
       </c>
       <c r="D23" t="n">
-        <v>-20282.2082995089</v>
+        <v>-10355.64194382899</v>
       </c>
       <c r="E23" t="n">
-        <v>7183.544266457749</v>
+        <v>-87371.41873951012</v>
       </c>
     </row>
     <row r="24">
@@ -2317,16 +2317,16 @@
         <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>54448.00000000005</v>
+        <v>-14901.99999999995</v>
       </c>
       <c r="C24" t="n">
-        <v>22530.62457977064</v>
+        <v>1104.423770277732</v>
       </c>
       <c r="D24" t="n">
-        <v>-20727.93591074153</v>
+        <v>-10801.36955506163</v>
       </c>
       <c r="E24" t="n">
-        <v>56250.68866902916</v>
+        <v>-24598.94578478384</v>
       </c>
     </row>
     <row r="25">
@@ -2334,16 +2334,16 @@
         <v>43</v>
       </c>
       <c r="B25" t="n">
-        <v>88478.00000000004</v>
+        <v>22353.00000000005</v>
       </c>
       <c r="C25" t="n">
-        <v>38013.49659357476</v>
+        <v>27067.62433623686</v>
       </c>
       <c r="D25" t="n">
-        <v>-20958.13699519985</v>
+        <v>-11031.57063951994</v>
       </c>
       <c r="E25" t="n">
-        <v>105533.359598375</v>
+        <v>38389.05369671697</v>
       </c>
     </row>
     <row r="26">
@@ -2351,16 +2351,16 @@
         <v>44</v>
       </c>
       <c r="B26" t="n">
-        <v>122508</v>
+        <v>59608.00000000005</v>
       </c>
       <c r="C26" t="n">
-        <v>53496.3686073788</v>
+        <v>53030.82490219583</v>
       </c>
       <c r="D26" t="n">
-        <v>-21073.10228926309</v>
+        <v>-11146.53593358318</v>
       </c>
       <c r="E26" t="n">
-        <v>154931.2663181158</v>
+        <v>101492.2889686127</v>
       </c>
     </row>
     <row r="27">
@@ -2368,16 +2368,16 @@
         <v>45</v>
       </c>
       <c r="B27" t="n">
-        <v>156538.0000000001</v>
+        <v>96863.00000000006</v>
       </c>
       <c r="C27" t="n">
-        <v>68979.24062118283</v>
+        <v>78994.02546815475</v>
       </c>
       <c r="D27" t="n">
-        <v>-21128.74285807236</v>
+        <v>-11202.17650239245</v>
       </c>
       <c r="E27" t="n">
-        <v>204388.4977631105</v>
+        <v>164654.8489657624</v>
       </c>
     </row>
   </sheetData>
@@ -2431,16 +2431,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-694212</v>
+        <v>-834512</v>
       </c>
       <c r="C2" t="n">
-        <v>-318967.9386628635</v>
+        <v>-571785.8773257269</v>
       </c>
       <c r="D2" t="n">
-        <v>1125606.069114531</v>
+        <v>1135532.635470211</v>
       </c>
       <c r="E2" t="n">
-        <v>112426.1304516675</v>
+        <v>-270765.2418555159</v>
       </c>
     </row>
     <row r="3">
@@ -2448,16 +2448,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-660182</v>
+        <v>-797257</v>
       </c>
       <c r="C3" t="n">
-        <v>-303528.8355960067</v>
+        <v>-545907.6711920134</v>
       </c>
       <c r="D3" t="n">
-        <v>1025606.069114531</v>
+        <v>1035532.635470211</v>
       </c>
       <c r="E3" t="n">
-        <v>61895.23351852456</v>
+        <v>-307632.0357218024</v>
       </c>
     </row>
     <row r="4">
@@ -2465,16 +2465,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-626152</v>
+        <v>-760002</v>
       </c>
       <c r="C4" t="n">
-        <v>-288089.7325291499</v>
+        <v>-520029.4650582997</v>
       </c>
       <c r="D4" t="n">
-        <v>925606.0691145463</v>
+        <v>935532.6354702262</v>
       </c>
       <c r="E4" t="n">
-        <v>11364.33658539644</v>
+        <v>-344498.8295880735</v>
       </c>
     </row>
     <row r="5">
@@ -2482,16 +2482,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-592122</v>
+        <v>-722747</v>
       </c>
       <c r="C5" t="n">
-        <v>-272650.629462293</v>
+        <v>-494151.258924586</v>
       </c>
       <c r="D5" t="n">
-        <v>825606.0691176662</v>
+        <v>835532.6354733461</v>
       </c>
       <c r="E5" t="n">
-        <v>-39166.56034462678</v>
+        <v>-381365.6234512399</v>
       </c>
     </row>
     <row r="6">
@@ -2499,16 +2499,16 @@
         <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>-558092</v>
+        <v>-685492</v>
       </c>
       <c r="C6" t="n">
-        <v>-257211.5263954362</v>
+        <v>-468273.0527908724</v>
       </c>
       <c r="D6" t="n">
-        <v>725606.0694146948</v>
+        <v>735532.6357703747</v>
       </c>
       <c r="E6" t="n">
-        <v>-89697.45698074135</v>
+        <v>-418232.4170204976</v>
       </c>
     </row>
     <row r="7">
@@ -2516,16 +2516,16 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>-524061.9999999999</v>
+        <v>-648237</v>
       </c>
       <c r="C7" t="n">
-        <v>-241772.4233285794</v>
+        <v>-442394.8466571587</v>
       </c>
       <c r="D7" t="n">
-        <v>625606.0838273054</v>
+        <v>635532.6501829851</v>
       </c>
       <c r="E7" t="n">
-        <v>-140228.3395012739</v>
+        <v>-455099.1964741737</v>
       </c>
     </row>
     <row r="8">
@@ -2533,16 +2533,16 @@
         <v>26</v>
       </c>
       <c r="B8" t="n">
-        <v>-490031.9999999999</v>
+        <v>-610982</v>
       </c>
       <c r="C8" t="n">
-        <v>-226333.3202617225</v>
+        <v>-416516.6405234451</v>
       </c>
       <c r="D8" t="n">
-        <v>525606.467856646</v>
+        <v>535533.0342123259</v>
       </c>
       <c r="E8" t="n">
-        <v>-190758.8524050764</v>
+        <v>-491965.6063111192</v>
       </c>
     </row>
     <row r="9">
@@ -2550,16 +2550,16 @@
         <v>27</v>
       </c>
       <c r="B9" t="n">
-        <v>-456001.9999999999</v>
+        <v>-573727</v>
       </c>
       <c r="C9" t="n">
-        <v>-210894.2171948657</v>
+        <v>-390638.4343897314</v>
       </c>
       <c r="D9" t="n">
-        <v>425612.4649126929</v>
+        <v>435539.0312683728</v>
       </c>
       <c r="E9" t="n">
-        <v>-241283.7522821728</v>
+        <v>-528826.4031213586</v>
       </c>
     </row>
     <row r="10">
@@ -2567,16 +2567,16 @@
         <v>28</v>
       </c>
       <c r="B10" t="n">
-        <v>-421971.9999999999</v>
+        <v>-536472</v>
       </c>
       <c r="C10" t="n">
-        <v>-195455.1141280089</v>
+        <v>-364760.2282560178</v>
       </c>
       <c r="D10" t="n">
-        <v>325670.5993240419</v>
+        <v>335597.1656797217</v>
       </c>
       <c r="E10" t="n">
-        <v>-291756.514803967</v>
+        <v>-565635.062576296</v>
       </c>
     </row>
     <row r="11">
@@ -2584,16 +2584,16 @@
         <v>29</v>
       </c>
       <c r="B11" t="n">
-        <v>-387941.9999999999</v>
+        <v>-499216.9999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-180016.0110611521</v>
+        <v>-338882.0221223042</v>
       </c>
       <c r="D11" t="n">
-        <v>226038.9412485755</v>
+        <v>235965.5076042553</v>
       </c>
       <c r="E11" t="n">
-        <v>-341919.0698125765</v>
+        <v>-602133.5145180488</v>
       </c>
     </row>
     <row r="12">
@@ -2601,16 +2601,16 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>-353911.9999999999</v>
+        <v>-461961.9999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>-164576.9079942952</v>
+        <v>-313003.8159885905</v>
       </c>
       <c r="D12" t="n">
-        <v>127638.1777258831</v>
+        <v>137564.744081563</v>
       </c>
       <c r="E12" t="n">
-        <v>-390850.7302684121</v>
+        <v>-637401.0719070275</v>
       </c>
     </row>
     <row r="13">
@@ -2618,16 +2618,16 @@
         <v>31</v>
       </c>
       <c r="B13" t="n">
-        <v>-319881.9999999999</v>
+        <v>-424706.9999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>-149137.8049274384</v>
+        <v>-287125.6098548768</v>
       </c>
       <c r="D13" t="n">
-        <v>82612.44206503418</v>
+        <v>92539.00842071408</v>
       </c>
       <c r="E13" t="n">
-        <v>-386407.3628624041</v>
+        <v>-619293.6014341627</v>
       </c>
     </row>
     <row r="14">
@@ -2635,16 +2635,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="n">
-        <v>-285851.9999999999</v>
+        <v>-387451.9999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-133698.7018605816</v>
+        <v>-261247.4037211632</v>
       </c>
       <c r="D14" t="n">
-        <v>44186.15143850625</v>
+        <v>54112.71779418615</v>
       </c>
       <c r="E14" t="n">
-        <v>-375364.5504220753</v>
+        <v>-594586.6859269768</v>
       </c>
     </row>
     <row r="15">
@@ -2652,16 +2652,16 @@
         <v>33</v>
       </c>
       <c r="B15" t="n">
-        <v>-251821.9999999999</v>
+        <v>-350196.9999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-118259.5987937248</v>
+        <v>-235369.1975874496</v>
       </c>
       <c r="D15" t="n">
-        <v>15225.27984709874</v>
+        <v>25151.84620277865</v>
       </c>
       <c r="E15" t="n">
-        <v>-354856.318946626</v>
+        <v>-560414.3513846709</v>
       </c>
     </row>
     <row r="16">
@@ -2669,16 +2669,16 @@
         <v>34</v>
       </c>
       <c r="B16" t="n">
-        <v>-217791.9999999999</v>
+        <v>-312941.9999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>-102820.495726868</v>
+        <v>-209490.991453736</v>
       </c>
       <c r="D16" t="n">
-        <v>-3522.26071946275</v>
+        <v>6404.305636217156</v>
       </c>
       <c r="E16" t="n">
-        <v>-324134.7564463307</v>
+        <v>-516028.6858175187</v>
       </c>
     </row>
     <row r="17">
@@ -2686,16 +2686,16 @@
         <v>35</v>
       </c>
       <c r="B17" t="n">
-        <v>-183761.9999999999</v>
+        <v>-275686.9999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>-87381.39266001113</v>
+        <v>-183612.7853200223</v>
       </c>
       <c r="D17" t="n">
-        <v>-13787.36662921808</v>
+        <v>-3860.800273538178</v>
       </c>
       <c r="E17" t="n">
-        <v>-284930.7592892292</v>
+        <v>-463160.5855935604</v>
       </c>
     </row>
     <row r="18">
@@ -2703,16 +2703,16 @@
         <v>36</v>
       </c>
       <c r="B18" t="n">
-        <v>-149731.9999999999</v>
+        <v>-238431.9999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>-71942.28959315433</v>
+        <v>-157734.5791863087</v>
       </c>
       <c r="D18" t="n">
-        <v>-18516.3558456546</v>
+        <v>-8589.789489974697</v>
       </c>
       <c r="E18" t="n">
-        <v>-240190.6454388089</v>
+        <v>-404756.3686762833</v>
       </c>
     </row>
     <row r="19">
@@ -2720,16 +2720,16 @@
         <v>37</v>
       </c>
       <c r="B19" t="n">
-        <v>-115702</v>
+        <v>-201176.9999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>-56503.18652629742</v>
+        <v>-131856.3730525948</v>
       </c>
       <c r="D19" t="n">
-        <v>-20351.90529912181</v>
+        <v>-10425.33894344191</v>
       </c>
       <c r="E19" t="n">
-        <v>-192557.0918254192</v>
+        <v>-343458.7119960367</v>
       </c>
     </row>
     <row r="20">
@@ -2737,16 +2737,16 @@
         <v>38</v>
       </c>
       <c r="B20" t="n">
-        <v>-81671.99999999996</v>
+        <v>-163921.9999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>-41064.08345944062</v>
+        <v>-105978.1669188812</v>
       </c>
       <c r="D20" t="n">
-        <v>-20955.43045780783</v>
+        <v>-11028.86410212793</v>
       </c>
       <c r="E20" t="n">
-        <v>-143691.5139172484</v>
+        <v>-280929.0310210091</v>
       </c>
     </row>
     <row r="21">
@@ -2754,16 +2754,16 @@
         <v>39</v>
       </c>
       <c r="B21" t="n">
-        <v>-47641.99999999995</v>
+        <v>-126666.9999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>-25624.98039258382</v>
+        <v>-80099.96078516764</v>
       </c>
       <c r="D21" t="n">
-        <v>-21124.79978557712</v>
+        <v>-11198.23342989721</v>
       </c>
       <c r="E21" t="n">
-        <v>-94391.78017816087</v>
+        <v>-217965.1942150648</v>
       </c>
     </row>
     <row r="22">
@@ -2771,16 +2771,16 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>-13611.99999999995</v>
+        <v>-89411.99999999994</v>
       </c>
       <c r="C22" t="n">
-        <v>-10185.87732572696</v>
+        <v>-54221.75465145393</v>
       </c>
       <c r="D22" t="n">
-        <v>-21165.71746867325</v>
+        <v>-11239.15111299335</v>
       </c>
       <c r="E22" t="n">
-        <v>-44963.59479440017</v>
+        <v>-154872.9057644472</v>
       </c>
     </row>
     <row r="23">
@@ -2788,16 +2788,16 @@
         <v>41</v>
       </c>
       <c r="B23" t="n">
-        <v>20418.00000000005</v>
+        <v>-52156.99999999995</v>
       </c>
       <c r="C23" t="n">
-        <v>5253.225741129834</v>
+        <v>-28343.54851774033</v>
       </c>
       <c r="D23" t="n">
-        <v>-21174.30375678555</v>
+        <v>-11247.73740110564</v>
       </c>
       <c r="E23" t="n">
-        <v>4496.921984344332</v>
+        <v>-91748.28591884591</v>
       </c>
     </row>
     <row r="24">
@@ -2805,16 +2805,16 @@
         <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>54448.00000000005</v>
+        <v>-14901.99999999995</v>
       </c>
       <c r="C24" t="n">
-        <v>20692.32880798663</v>
+        <v>-2465.342384026735</v>
       </c>
       <c r="D24" t="n">
-        <v>-21175.8827586159</v>
+        <v>-11249.316402936</v>
       </c>
       <c r="E24" t="n">
-        <v>53964.44604937079</v>
+        <v>-28616.65878696268</v>
       </c>
     </row>
     <row r="25">
@@ -2822,16 +2822,16 @@
         <v>43</v>
       </c>
       <c r="B25" t="n">
-        <v>88478.00000000004</v>
+        <v>22353.00000000005</v>
       </c>
       <c r="C25" t="n">
-        <v>36131.43187484343</v>
+        <v>23412.86374968686</v>
       </c>
       <c r="D25" t="n">
-        <v>-21176.13943948973</v>
+        <v>-11249.57308380982</v>
       </c>
       <c r="E25" t="n">
-        <v>103433.2924353538</v>
+        <v>34516.2906658771</v>
       </c>
     </row>
     <row r="26">
@@ -2839,16 +2839,16 @@
         <v>44</v>
       </c>
       <c r="B26" t="n">
-        <v>122508</v>
+        <v>59608.00000000005</v>
       </c>
       <c r="C26" t="n">
-        <v>51570.53494170035</v>
+        <v>49291.06988340069</v>
       </c>
       <c r="D26" t="n">
-        <v>-21176.17662921157</v>
+        <v>-11249.61027353167</v>
       </c>
       <c r="E26" t="n">
-        <v>152902.3583124888</v>
+        <v>97649.45960986908</v>
       </c>
     </row>
     <row r="27">
@@ -2856,16 +2856,16 @@
         <v>45</v>
       </c>
       <c r="B27" t="n">
-        <v>156538.0000000001</v>
+        <v>96863.00000000006</v>
       </c>
       <c r="C27" t="n">
-        <v>67009.63800855714</v>
+        <v>75169.27601711429</v>
       </c>
       <c r="D27" t="n">
-        <v>-21176.18146941869</v>
+        <v>-11249.61511373879</v>
       </c>
       <c r="E27" t="n">
-        <v>202371.4565391385</v>
+        <v>160782.6609033756</v>
       </c>
     </row>
   </sheetData>
@@ -2919,16 +2919,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-694212</v>
+        <v>-834512</v>
       </c>
       <c r="C2" t="n">
-        <v>-319762.7631005452</v>
+        <v>-573375.5262010903</v>
       </c>
       <c r="D2" t="n">
-        <v>1128823.817892751</v>
+        <v>1138750.38424843</v>
       </c>
       <c r="E2" t="n">
-        <v>114849.0547922056</v>
+        <v>-269137.1419526599</v>
       </c>
     </row>
     <row r="3">
@@ -2936,16 +2936,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-660182</v>
+        <v>-797257</v>
       </c>
       <c r="C3" t="n">
-        <v>-304363.4012555724</v>
+        <v>-547576.8025111448</v>
       </c>
       <c r="D3" t="n">
-        <v>1028823.817892751</v>
+        <v>1038750.38424843</v>
       </c>
       <c r="E3" t="n">
-        <v>64278.41663717816</v>
+        <v>-306083.4182627144</v>
       </c>
     </row>
     <row r="4">
@@ -2953,16 +2953,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-626152</v>
+        <v>-760002</v>
       </c>
       <c r="C4" t="n">
-        <v>-288964.0394105997</v>
+        <v>-521778.0788211994</v>
       </c>
       <c r="D4" t="n">
-        <v>928823.8178927505</v>
+        <v>938750.3842484304</v>
       </c>
       <c r="E4" t="n">
-        <v>13707.77848215075</v>
+        <v>-343029.6945727691</v>
       </c>
     </row>
     <row r="5">
@@ -2970,16 +2970,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-592122</v>
+        <v>-722747</v>
       </c>
       <c r="C5" t="n">
-        <v>-273564.6775656269</v>
+        <v>-495979.3551312538</v>
       </c>
       <c r="D5" t="n">
-        <v>828823.8178927505</v>
+        <v>838750.3842484304</v>
       </c>
       <c r="E5" t="n">
-        <v>-36862.85967287642</v>
+        <v>-379975.9708828235</v>
       </c>
     </row>
     <row r="6">
@@ -2987,16 +2987,16 @@
         <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>-558092</v>
+        <v>-685492</v>
       </c>
       <c r="C6" t="n">
-        <v>-258165.3157206542</v>
+        <v>-470180.6314413083</v>
       </c>
       <c r="D6" t="n">
-        <v>728823.8178927505</v>
+        <v>738750.3842484304</v>
       </c>
       <c r="E6" t="n">
-        <v>-87433.4978279036</v>
+        <v>-416922.2471928778</v>
       </c>
     </row>
     <row r="7">
@@ -3004,16 +3004,16 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>-524061.9999999999</v>
+        <v>-648237</v>
       </c>
       <c r="C7" t="n">
-        <v>-242765.9538756814</v>
+        <v>-444381.9077513628</v>
       </c>
       <c r="D7" t="n">
-        <v>628823.8178927506</v>
+        <v>638750.3842484305</v>
       </c>
       <c r="E7" t="n">
-        <v>-138004.1359829308</v>
+        <v>-453868.5235029323</v>
       </c>
     </row>
     <row r="8">
@@ -3021,16 +3021,16 @@
         <v>26</v>
       </c>
       <c r="B8" t="n">
-        <v>-490031.9999999999</v>
+        <v>-610982</v>
       </c>
       <c r="C8" t="n">
-        <v>-227366.5920307087</v>
+        <v>-418583.1840614174</v>
       </c>
       <c r="D8" t="n">
-        <v>528823.8178927506</v>
+        <v>538750.3842484305</v>
       </c>
       <c r="E8" t="n">
-        <v>-188574.7741379581</v>
+        <v>-490814.7998129869</v>
       </c>
     </row>
     <row r="9">
@@ -3038,16 +3038,16 @@
         <v>27</v>
       </c>
       <c r="B9" t="n">
-        <v>-456001.9999999999</v>
+        <v>-573727</v>
       </c>
       <c r="C9" t="n">
-        <v>-211967.230185736</v>
+        <v>-392784.4603714719</v>
       </c>
       <c r="D9" t="n">
-        <v>428823.8178927506</v>
+        <v>438750.3842484305</v>
       </c>
       <c r="E9" t="n">
-        <v>-239145.4122929854</v>
+        <v>-527761.0761230415</v>
       </c>
     </row>
     <row r="10">
@@ -3055,16 +3055,16 @@
         <v>28</v>
       </c>
       <c r="B10" t="n">
-        <v>-421971.9999999999</v>
+        <v>-536472</v>
       </c>
       <c r="C10" t="n">
-        <v>-196567.8683407632</v>
+        <v>-366985.7366815264</v>
       </c>
       <c r="D10" t="n">
-        <v>328823.8178927506</v>
+        <v>338750.3842484305</v>
       </c>
       <c r="E10" t="n">
-        <v>-289716.0504480125</v>
+        <v>-564707.3524330959</v>
       </c>
     </row>
     <row r="11">
@@ -3072,16 +3072,16 @@
         <v>29</v>
       </c>
       <c r="B11" t="n">
-        <v>-387941.9999999999</v>
+        <v>-499216.9999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-181168.5064957904</v>
+        <v>-341187.0129915809</v>
       </c>
       <c r="D11" t="n">
-        <v>228823.8178927506</v>
+        <v>238750.3842484305</v>
       </c>
       <c r="E11" t="n">
-        <v>-340286.6886030397</v>
+        <v>-601653.6287431504</v>
       </c>
     </row>
     <row r="12">
@@ -3089,16 +3089,16 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>-353911.9999999999</v>
+        <v>-461961.9999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>-165769.1446508177</v>
+        <v>-315388.2893016355</v>
       </c>
       <c r="D12" t="n">
-        <v>128823.8178927506</v>
+        <v>138750.3842484305</v>
       </c>
       <c r="E12" t="n">
-        <v>-390857.3267580671</v>
+        <v>-638599.905053205</v>
       </c>
     </row>
     <row r="13">
@@ -3106,16 +3106,16 @@
         <v>31</v>
       </c>
       <c r="B13" t="n">
-        <v>-319881.9999999999</v>
+        <v>-424706.9999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>-150369.7828058449</v>
+        <v>-289589.5656116898</v>
       </c>
       <c r="D13" t="n">
-        <v>78823.81789275059</v>
+        <v>88750.38424843049</v>
       </c>
       <c r="E13" t="n">
-        <v>-391427.9649130942</v>
+        <v>-625546.1813632593</v>
       </c>
     </row>
     <row r="14">
@@ -3123,16 +3123,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="n">
-        <v>-285851.9999999999</v>
+        <v>-387451.9999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-134970.4209608722</v>
+        <v>-263790.8419217444</v>
       </c>
       <c r="D14" t="n">
-        <v>28823.8178927506</v>
+        <v>38750.38424843051</v>
       </c>
       <c r="E14" t="n">
-        <v>-391998.6030681215</v>
+        <v>-612492.4576733139</v>
       </c>
     </row>
     <row r="15">
@@ -3140,16 +3140,16 @@
         <v>33</v>
       </c>
       <c r="B15" t="n">
-        <v>-251821.9999999999</v>
+        <v>-350196.9999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-119571.0591158995</v>
+        <v>-237992.118231799</v>
       </c>
       <c r="D15" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E15" t="n">
-        <v>-392569.2412231488</v>
+        <v>-599438.7339833685</v>
       </c>
     </row>
     <row r="16">
@@ -3157,16 +3157,16 @@
         <v>34</v>
       </c>
       <c r="B16" t="n">
-        <v>-217791.9999999999</v>
+        <v>-312941.9999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>-104171.6972709267</v>
+        <v>-212193.3945418535</v>
       </c>
       <c r="D16" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E16" t="n">
-        <v>-343139.8793781761</v>
+        <v>-536385.0102934228</v>
       </c>
     </row>
     <row r="17">
@@ -3174,16 +3174,16 @@
         <v>35</v>
       </c>
       <c r="B17" t="n">
-        <v>-183761.9999999999</v>
+        <v>-275686.9999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>-88772.33542595402</v>
+        <v>-186394.670851908</v>
       </c>
       <c r="D17" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E17" t="n">
-        <v>-293710.5175332034</v>
+        <v>-473331.2866034775</v>
       </c>
     </row>
     <row r="18">
@@ -3191,16 +3191,16 @@
         <v>36</v>
       </c>
       <c r="B18" t="n">
-        <v>-149731.9999999999</v>
+        <v>-238431.9999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>-73372.9735809812</v>
+        <v>-160595.9471619624</v>
       </c>
       <c r="D18" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E18" t="n">
-        <v>-244281.1556882305</v>
+        <v>-410277.5629135318</v>
       </c>
     </row>
     <row r="19">
@@ -3208,16 +3208,16 @@
         <v>37</v>
       </c>
       <c r="B19" t="n">
-        <v>-115702</v>
+        <v>-201176.9999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>-57973.61173600849</v>
+        <v>-134797.223472017</v>
       </c>
       <c r="D19" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E19" t="n">
-        <v>-194851.7938432578</v>
+        <v>-347223.8392235864</v>
       </c>
     </row>
     <row r="20">
@@ -3225,16 +3225,16 @@
         <v>38</v>
       </c>
       <c r="B20" t="n">
-        <v>-81671.99999999996</v>
+        <v>-163921.9999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>-42574.24989103578</v>
+        <v>-108998.4997820716</v>
       </c>
       <c r="D20" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E20" t="n">
-        <v>-145422.4319982851</v>
+        <v>-284170.115533641</v>
       </c>
     </row>
     <row r="21">
@@ -3242,16 +3242,16 @@
         <v>39</v>
       </c>
       <c r="B21" t="n">
-        <v>-47641.99999999995</v>
+        <v>-126666.9999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>-27174.88804606302</v>
+        <v>-83199.77609212603</v>
       </c>
       <c r="D21" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E21" t="n">
-        <v>-95993.07015331236</v>
+        <v>-221116.3918436955</v>
       </c>
     </row>
     <row r="22">
@@ -3259,16 +3259,16 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>-13611.99999999995</v>
+        <v>-89411.99999999994</v>
       </c>
       <c r="C22" t="n">
-        <v>-11775.52620109025</v>
+        <v>-57401.0524021805</v>
       </c>
       <c r="D22" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E22" t="n">
-        <v>-46563.7083083396</v>
+        <v>-158062.66815375</v>
       </c>
     </row>
     <row r="23">
@@ -3276,16 +3276,16 @@
         <v>41</v>
       </c>
       <c r="B23" t="n">
-        <v>20418.00000000005</v>
+        <v>-52156.99999999995</v>
       </c>
       <c r="C23" t="n">
-        <v>3623.835643882456</v>
+        <v>-31602.32871223509</v>
       </c>
       <c r="D23" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E23" t="n">
-        <v>2865.653536633101</v>
+        <v>-95008.94446380452</v>
       </c>
     </row>
     <row r="24">
@@ -3293,16 +3293,16 @@
         <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>54448.00000000005</v>
+        <v>-14901.99999999995</v>
       </c>
       <c r="C24" t="n">
-        <v>19023.19748885522</v>
+        <v>-5803.605022289557</v>
       </c>
       <c r="D24" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E24" t="n">
-        <v>52295.01538160587</v>
+        <v>-31955.220773859</v>
       </c>
     </row>
     <row r="25">
@@ -3310,16 +3310,16 @@
         <v>43</v>
       </c>
       <c r="B25" t="n">
-        <v>88478.00000000004</v>
+        <v>22353.00000000005</v>
       </c>
       <c r="C25" t="n">
-        <v>34422.55933382793</v>
+        <v>19995.11866765586</v>
       </c>
       <c r="D25" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E25" t="n">
-        <v>101724.3772265786</v>
+        <v>31098.50291608642</v>
       </c>
     </row>
     <row r="26">
@@ -3327,16 +3327,16 @@
         <v>44</v>
       </c>
       <c r="B26" t="n">
-        <v>122508</v>
+        <v>59608.00000000005</v>
       </c>
       <c r="C26" t="n">
-        <v>49821.92117880064</v>
+        <v>45793.84235760127</v>
       </c>
       <c r="D26" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E26" t="n">
-        <v>151153.7390715513</v>
+        <v>94152.22660603184</v>
       </c>
     </row>
     <row r="27">
@@ -3344,16 +3344,16 @@
         <v>45</v>
       </c>
       <c r="B27" t="n">
-        <v>156538.0000000001</v>
+        <v>96863.00000000006</v>
       </c>
       <c r="C27" t="n">
-        <v>65221.28302377346</v>
+        <v>71592.56604754692</v>
       </c>
       <c r="D27" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E27" t="n">
-        <v>200583.1009165241</v>
+        <v>157205.9502959775</v>
       </c>
     </row>
   </sheetData>
@@ -3407,16 +3407,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-694212</v>
+        <v>-834512</v>
       </c>
       <c r="C2" t="n">
-        <v>-320580.9029836912</v>
+        <v>-575011.8059673824</v>
       </c>
       <c r="D2" t="n">
-        <v>1128823.817892751</v>
+        <v>1138750.38424843</v>
       </c>
       <c r="E2" t="n">
-        <v>114030.9149090595</v>
+        <v>-270773.421718952</v>
       </c>
     </row>
     <row r="3">
@@ -3424,16 +3424,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-660182</v>
+        <v>-797257</v>
       </c>
       <c r="C3" t="n">
-        <v>-305222.4481328757</v>
+        <v>-549294.8962657514</v>
       </c>
       <c r="D3" t="n">
-        <v>1028823.817892751</v>
+        <v>1038750.38424843</v>
       </c>
       <c r="E3" t="n">
-        <v>63419.36975987488</v>
+        <v>-307801.512017321</v>
       </c>
     </row>
     <row r="4">
@@ -3441,16 +3441,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-626152</v>
+        <v>-760002</v>
       </c>
       <c r="C4" t="n">
-        <v>-289863.9932820603</v>
+        <v>-523577.9865641206</v>
       </c>
       <c r="D4" t="n">
-        <v>928823.8178927505</v>
+        <v>938750.3842484304</v>
       </c>
       <c r="E4" t="n">
-        <v>12807.82461069024</v>
+        <v>-344829.6023156901</v>
       </c>
     </row>
     <row r="5">
@@ -3458,16 +3458,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-592122</v>
+        <v>-722747</v>
       </c>
       <c r="C5" t="n">
-        <v>-274505.5384312448</v>
+        <v>-497861.0768624897</v>
       </c>
       <c r="D5" t="n">
-        <v>828823.8178927505</v>
+        <v>838750.3842484304</v>
       </c>
       <c r="E5" t="n">
-        <v>-37803.72053849441</v>
+        <v>-381857.6926140594</v>
       </c>
     </row>
     <row r="6">
@@ -3475,16 +3475,16 @@
         <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>-558092</v>
+        <v>-685492</v>
       </c>
       <c r="C6" t="n">
-        <v>-259147.0835804294</v>
+        <v>-472144.1671608587</v>
       </c>
       <c r="D6" t="n">
-        <v>728823.8178927505</v>
+        <v>738750.3842484304</v>
       </c>
       <c r="E6" t="n">
-        <v>-88415.26568767894</v>
+        <v>-418885.7829124285</v>
       </c>
     </row>
     <row r="7">
@@ -3492,16 +3492,16 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>-524061.9999999999</v>
+        <v>-648237</v>
       </c>
       <c r="C7" t="n">
-        <v>-243788.628729614</v>
+        <v>-446427.2574592279</v>
       </c>
       <c r="D7" t="n">
-        <v>628823.8178927506</v>
+        <v>638750.3842484305</v>
       </c>
       <c r="E7" t="n">
-        <v>-139026.8108368634</v>
+        <v>-455913.8732107974</v>
       </c>
     </row>
     <row r="8">
@@ -3509,16 +3509,16 @@
         <v>26</v>
       </c>
       <c r="B8" t="n">
-        <v>-490031.9999999999</v>
+        <v>-610982</v>
       </c>
       <c r="C8" t="n">
-        <v>-228430.1738787985</v>
+        <v>-420710.347757597</v>
       </c>
       <c r="D8" t="n">
-        <v>528823.8178927506</v>
+        <v>538750.3842484305</v>
       </c>
       <c r="E8" t="n">
-        <v>-189638.3559860479</v>
+        <v>-492941.9635091665</v>
       </c>
     </row>
     <row r="9">
@@ -3526,16 +3526,16 @@
         <v>27</v>
       </c>
       <c r="B9" t="n">
-        <v>-456001.9999999999</v>
+        <v>-573727</v>
       </c>
       <c r="C9" t="n">
-        <v>-213071.7190279831</v>
+        <v>-394993.4380559662</v>
       </c>
       <c r="D9" t="n">
-        <v>428823.8178927506</v>
+        <v>438750.3842484305</v>
       </c>
       <c r="E9" t="n">
-        <v>-240249.9011352324</v>
+        <v>-529970.0538075357</v>
       </c>
     </row>
     <row r="10">
@@ -3543,16 +3543,16 @@
         <v>28</v>
       </c>
       <c r="B10" t="n">
-        <v>-421971.9999999999</v>
+        <v>-536472</v>
       </c>
       <c r="C10" t="n">
-        <v>-197713.2641771676</v>
+        <v>-369276.5283543352</v>
       </c>
       <c r="D10" t="n">
-        <v>328823.8178927506</v>
+        <v>338750.3842484305</v>
       </c>
       <c r="E10" t="n">
-        <v>-290861.4462844169</v>
+        <v>-566998.1441059047</v>
       </c>
     </row>
     <row r="11">
@@ -3560,16 +3560,16 @@
         <v>29</v>
       </c>
       <c r="B11" t="n">
-        <v>-387941.9999999999</v>
+        <v>-499216.9999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-182354.8093263522</v>
+        <v>-343559.6186527044</v>
       </c>
       <c r="D11" t="n">
-        <v>228823.8178927506</v>
+        <v>238750.3842484305</v>
       </c>
       <c r="E11" t="n">
-        <v>-341472.9914336015</v>
+        <v>-604026.2344042739</v>
       </c>
     </row>
     <row r="12">
@@ -3577,16 +3577,16 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>-353911.9999999999</v>
+        <v>-461961.9999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>-166996.3544755368</v>
+        <v>-317842.7089510736</v>
       </c>
       <c r="D12" t="n">
-        <v>128823.8178927506</v>
+        <v>138750.3842484305</v>
       </c>
       <c r="E12" t="n">
-        <v>-392084.5365827861</v>
+        <v>-641054.324702643</v>
       </c>
     </row>
     <row r="13">
@@ -3594,16 +3594,16 @@
         <v>31</v>
       </c>
       <c r="B13" t="n">
-        <v>-319881.9999999999</v>
+        <v>-424706.9999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>-151637.8996247213</v>
+        <v>-292125.7992494426</v>
       </c>
       <c r="D13" t="n">
-        <v>78823.81789275059</v>
+        <v>88750.38424843049</v>
       </c>
       <c r="E13" t="n">
-        <v>-392696.0817319707</v>
+        <v>-628082.415001012</v>
       </c>
     </row>
     <row r="14">
@@ -3611,16 +3611,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="n">
-        <v>-285851.9999999999</v>
+        <v>-387451.9999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-136279.4447739059</v>
+        <v>-266408.8895478117</v>
       </c>
       <c r="D14" t="n">
-        <v>28823.8178927506</v>
+        <v>38750.38424843051</v>
       </c>
       <c r="E14" t="n">
-        <v>-393307.6268811552</v>
+        <v>-615110.5052993811</v>
       </c>
     </row>
     <row r="15">
@@ -3628,16 +3628,16 @@
         <v>33</v>
       </c>
       <c r="B15" t="n">
-        <v>-251821.9999999999</v>
+        <v>-350196.9999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-120920.9899230904</v>
+        <v>-240691.9798461809</v>
       </c>
       <c r="D15" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E15" t="n">
-        <v>-393919.1720303398</v>
+        <v>-602138.5955977504</v>
       </c>
     </row>
     <row r="16">
@@ -3645,16 +3645,16 @@
         <v>34</v>
       </c>
       <c r="B16" t="n">
-        <v>-217791.9999999999</v>
+        <v>-312941.9999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>-105562.535072275</v>
+        <v>-214975.0701445499</v>
       </c>
       <c r="D16" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E16" t="n">
-        <v>-344530.7171795243</v>
+        <v>-539166.6858961195</v>
       </c>
     </row>
     <row r="17">
@@ -3662,16 +3662,16 @@
         <v>35</v>
       </c>
       <c r="B17" t="n">
-        <v>-183761.9999999999</v>
+        <v>-275686.9999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>-90204.0802214595</v>
+        <v>-189258.160442919</v>
       </c>
       <c r="D17" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E17" t="n">
-        <v>-295142.2623287088</v>
+        <v>-476194.7761944885</v>
       </c>
     </row>
     <row r="18">
@@ -3679,16 +3679,16 @@
         <v>36</v>
       </c>
       <c r="B18" t="n">
-        <v>-149731.9999999999</v>
+        <v>-238431.9999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>-74845.62537064409</v>
+        <v>-163541.2507412882</v>
       </c>
       <c r="D18" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E18" t="n">
-        <v>-245753.8074778934</v>
+        <v>-413222.8664928576</v>
       </c>
     </row>
     <row r="19">
@@ -3696,16 +3696,16 @@
         <v>37</v>
       </c>
       <c r="B19" t="n">
-        <v>-115702</v>
+        <v>-201176.9999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>-59487.17051982862</v>
+        <v>-137824.3410396572</v>
       </c>
       <c r="D19" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E19" t="n">
-        <v>-196365.352627078</v>
+        <v>-350250.9567912267</v>
       </c>
     </row>
     <row r="20">
@@ -3713,16 +3713,16 @@
         <v>38</v>
       </c>
       <c r="B20" t="n">
-        <v>-81671.99999999996</v>
+        <v>-163921.9999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>-44128.71566901327</v>
+        <v>-112107.4313380265</v>
       </c>
       <c r="D20" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E20" t="n">
-        <v>-146976.8977762626</v>
+        <v>-287279.047089596</v>
       </c>
     </row>
     <row r="21">
@@ -3730,16 +3730,16 @@
         <v>39</v>
       </c>
       <c r="B21" t="n">
-        <v>-47641.99999999995</v>
+        <v>-126666.9999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>-28770.2608181978</v>
+        <v>-86390.5216363956</v>
       </c>
       <c r="D21" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E21" t="n">
-        <v>-97588.44292544715</v>
+        <v>-224307.137387965</v>
       </c>
     </row>
     <row r="22">
@@ -3747,16 +3747,16 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>-13611.99999999995</v>
+        <v>-89411.99999999994</v>
       </c>
       <c r="C22" t="n">
-        <v>-13411.80596738233</v>
+        <v>-60673.61193476466</v>
       </c>
       <c r="D22" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E22" t="n">
-        <v>-48199.98807463168</v>
+        <v>-161335.2276863341</v>
       </c>
     </row>
     <row r="23">
@@ -3764,16 +3764,16 @@
         <v>41</v>
       </c>
       <c r="B23" t="n">
-        <v>20418.00000000005</v>
+        <v>-52156.99999999995</v>
       </c>
       <c r="C23" t="n">
-        <v>1946.648883433081</v>
+        <v>-34956.70223313384</v>
       </c>
       <c r="D23" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E23" t="n">
-        <v>1188.466776183726</v>
+        <v>-98363.31798470327</v>
       </c>
     </row>
     <row r="24">
@@ -3781,16 +3781,16 @@
         <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>54448.00000000005</v>
+        <v>-14901.99999999995</v>
       </c>
       <c r="C24" t="n">
-        <v>17305.10373424855</v>
+        <v>-9239.792531502899</v>
       </c>
       <c r="D24" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E24" t="n">
-        <v>50576.9216269992</v>
+        <v>-35391.40828307235</v>
       </c>
     </row>
     <row r="25">
@@ -3798,16 +3798,16 @@
         <v>43</v>
       </c>
       <c r="B25" t="n">
-        <v>88478.00000000004</v>
+        <v>22353.00000000005</v>
       </c>
       <c r="C25" t="n">
-        <v>32663.55858506402</v>
+        <v>16477.11717012804</v>
       </c>
       <c r="D25" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E25" t="n">
-        <v>99965.37647781466</v>
+        <v>27580.5014185586</v>
       </c>
     </row>
     <row r="26">
@@ -3815,16 +3815,16 @@
         <v>44</v>
       </c>
       <c r="B26" t="n">
-        <v>122508</v>
+        <v>59608.00000000005</v>
       </c>
       <c r="C26" t="n">
-        <v>48022.01343587943</v>
+        <v>42194.02687175886</v>
       </c>
       <c r="D26" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E26" t="n">
-        <v>149353.8313286301</v>
+        <v>90552.41112018943</v>
       </c>
     </row>
     <row r="27">
@@ -3832,16 +3832,16 @@
         <v>45</v>
       </c>
       <c r="B27" t="n">
-        <v>156538.0000000001</v>
+        <v>96863.00000000006</v>
       </c>
       <c r="C27" t="n">
-        <v>63380.4682866949</v>
+        <v>67910.9365733898</v>
       </c>
       <c r="D27" t="n">
-        <v>-21176.1821072494</v>
+        <v>-11249.6157515695</v>
       </c>
       <c r="E27" t="n">
-        <v>198742.2861794456</v>
+        <v>153524.3208218204</v>
       </c>
     </row>
   </sheetData>
@@ -3895,16 +3895,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-694212</v>
+        <v>-834512</v>
       </c>
       <c r="C2" t="n">
-        <v>-315165.4256674917</v>
+        <v>-565177.4827832899</v>
       </c>
       <c r="D2" t="n">
-        <v>1086388.106268457</v>
+        <v>1096314.672624137</v>
       </c>
       <c r="E2" t="n">
-        <v>77010.68060096563</v>
+        <v>-303374.8101591526</v>
       </c>
     </row>
     <row r="3">
@@ -3912,16 +3912,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-660182</v>
+        <v>-797257</v>
       </c>
       <c r="C3" t="n">
-        <v>-299536.1969508663</v>
+        <v>-538968.8569224543</v>
       </c>
       <c r="D3" t="n">
-        <v>986811.9941812449</v>
+        <v>996738.5605369247</v>
       </c>
       <c r="E3" t="n">
-        <v>27093.79723037849</v>
+        <v>-339487.2963855295</v>
       </c>
     </row>
     <row r="4">
@@ -3929,16 +3929,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-626152</v>
+        <v>-760002</v>
       </c>
       <c r="C4" t="n">
-        <v>-283906.9682342409</v>
+        <v>-512760.2310616188</v>
       </c>
       <c r="D4" t="n">
-        <v>887843.8950403822</v>
+        <v>897770.461396062</v>
       </c>
       <c r="E4" t="n">
-        <v>-22215.07319385873</v>
+        <v>-374991.7696655567</v>
       </c>
     </row>
     <row r="5">
@@ -3946,16 +3946,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-592122</v>
+        <v>-722747</v>
       </c>
       <c r="C5" t="n">
-        <v>-268277.7395176155</v>
+        <v>-486551.6052007833</v>
       </c>
       <c r="D5" t="n">
-        <v>790059.6760477136</v>
+        <v>799986.2424033935</v>
       </c>
       <c r="E5" t="n">
-        <v>-70340.0634699018</v>
+        <v>-409312.3627973899</v>
       </c>
     </row>
     <row r="6">
@@ -3963,16 +3963,16 @@
         <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>-558092</v>
+        <v>-685492</v>
       </c>
       <c r="C6" t="n">
-        <v>-252648.5108009901</v>
+        <v>-460342.9793399479</v>
       </c>
       <c r="D6" t="n">
-        <v>694319.6891601172</v>
+        <v>704246.2555157971</v>
       </c>
       <c r="E6" t="n">
-        <v>-116420.8216408729</v>
+        <v>-441588.7238241509</v>
       </c>
     </row>
     <row r="7">
@@ -3980,16 +3980,16 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>-524061.9999999999</v>
+        <v>-648237</v>
       </c>
       <c r="C7" t="n">
-        <v>-237019.2820843646</v>
+        <v>-434134.3534791123</v>
       </c>
       <c r="D7" t="n">
-        <v>601751.7792792822</v>
+        <v>611678.3456349621</v>
       </c>
       <c r="E7" t="n">
-        <v>-159329.5028050824</v>
+        <v>-470693.0078441502</v>
       </c>
     </row>
     <row r="8">
@@ -3997,16 +3997,16 @@
         <v>26</v>
       </c>
       <c r="B8" t="n">
-        <v>-490031.9999999999</v>
+        <v>-610982</v>
       </c>
       <c r="C8" t="n">
-        <v>-221390.0533677392</v>
+        <v>-407925.7276182767</v>
       </c>
       <c r="D8" t="n">
-        <v>513659.911319979</v>
+        <v>523586.4776756589</v>
       </c>
       <c r="E8" t="n">
-        <v>-197762.1420477602</v>
+        <v>-495321.2499426178</v>
       </c>
     </row>
     <row r="9">
@@ -4014,16 +4014,16 @@
         <v>27</v>
       </c>
       <c r="B9" t="n">
-        <v>-456001.9999999999</v>
+        <v>-573727</v>
       </c>
       <c r="C9" t="n">
-        <v>-205760.8246511138</v>
+        <v>-381717.1017574412</v>
       </c>
       <c r="D9" t="n">
-        <v>431372.7320503047</v>
+        <v>441299.2984059845</v>
       </c>
       <c r="E9" t="n">
-        <v>-230390.0926008091</v>
+        <v>-514144.8033514566</v>
       </c>
     </row>
     <row r="10">
@@ -4031,16 +4031,16 @@
         <v>28</v>
       </c>
       <c r="B10" t="n">
-        <v>-421971.9999999999</v>
+        <v>-536472</v>
       </c>
       <c r="C10" t="n">
-        <v>-190131.5959344884</v>
+        <v>-355508.4758966058</v>
       </c>
       <c r="D10" t="n">
-        <v>356069.690081095</v>
+        <v>365996.2564367749</v>
       </c>
       <c r="E10" t="n">
-        <v>-256033.9058533934</v>
+        <v>-525984.2194598309</v>
       </c>
     </row>
     <row r="11">
@@ -4048,16 +4048,16 @@
         <v>29</v>
       </c>
       <c r="B11" t="n">
-        <v>-387941.9999999999</v>
+        <v>-499216.9999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-174502.3672178629</v>
+        <v>-329299.8500357702</v>
       </c>
       <c r="D11" t="n">
-        <v>288629.6156713821</v>
+        <v>298556.1820270619</v>
       </c>
       <c r="E11" t="n">
-        <v>-273814.7515464808</v>
+        <v>-529960.6680087082</v>
       </c>
     </row>
     <row r="12">
@@ -4065,16 +4065,16 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>-353911.9999999999</v>
+        <v>-461961.9999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>-158873.1385012376</v>
+        <v>-303091.2241749348</v>
       </c>
       <c r="D12" t="n">
-        <v>229536.2982407009</v>
+        <v>239462.8645963809</v>
       </c>
       <c r="E12" t="n">
-        <v>-283248.8402605365</v>
+        <v>-525590.3595785538</v>
       </c>
     </row>
     <row r="13">
@@ -4082,16 +4082,16 @@
         <v>31</v>
       </c>
       <c r="B13" t="n">
-        <v>-319881.9999999999</v>
+        <v>-424706.9999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>-143243.9097846122</v>
+        <v>-276882.5983140994</v>
       </c>
       <c r="D13" t="n">
-        <v>178854.8627365353</v>
+        <v>188781.4290922153</v>
       </c>
       <c r="E13" t="n">
-        <v>-284271.0470480768</v>
+        <v>-512808.169221884</v>
       </c>
     </row>
     <row r="14">
@@ -4099,16 +4099,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="n">
-        <v>-285851.9999999999</v>
+        <v>-387451.9999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>-127614.6810679868</v>
+        <v>-250673.9724532638</v>
       </c>
       <c r="D14" t="n">
-        <v>136271.870889834</v>
+        <v>146198.4372455139</v>
       </c>
       <c r="E14" t="n">
-        <v>-277194.8101781528</v>
+        <v>-491927.5352077498</v>
       </c>
     </row>
     <row r="15">
@@ -4116,16 +4116,16 @@
         <v>33</v>
       </c>
       <c r="B15" t="n">
-        <v>-251821.9999999999</v>
+        <v>-350196.9999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-111985.4523513613</v>
+        <v>-224465.3465924282</v>
       </c>
       <c r="D15" t="n">
-        <v>101178.5009907308</v>
+        <v>111105.0673464107</v>
       </c>
       <c r="E15" t="n">
-        <v>-262628.9513606305</v>
+        <v>-463557.2792460175</v>
       </c>
     </row>
     <row r="16">
@@ -4133,16 +4133,16 @@
         <v>34</v>
       </c>
       <c r="B16" t="n">
-        <v>-217791.9999999999</v>
+        <v>-312941.9999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>-96356.22363473588</v>
+        <v>-198256.7207315926</v>
       </c>
       <c r="D16" t="n">
-        <v>72772.14631523409</v>
+        <v>82698.71267091398</v>
       </c>
       <c r="E16" t="n">
-        <v>-241376.0773195017</v>
+        <v>-428500.0080606786</v>
       </c>
     </row>
     <row r="17">
@@ -4150,16 +4150,16 @@
         <v>35</v>
       </c>
       <c r="B17" t="n">
-        <v>-183761.9999999999</v>
+        <v>-275686.9999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>-80726.99491811046</v>
+        <v>-172048.0948707571</v>
       </c>
       <c r="D17" t="n">
-        <v>50155.33642707163</v>
+        <v>60081.90278275152</v>
       </c>
       <c r="E17" t="n">
-        <v>-214333.6584910388</v>
+        <v>-387653.1920880055</v>
       </c>
     </row>
     <row r="18">
@@ -4167,16 +4167,16 @@
         <v>36</v>
       </c>
       <c r="B18" t="n">
-        <v>-149731.9999999999</v>
+        <v>-238431.9999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>-65097.76620148512</v>
+        <v>-145839.4690099218</v>
       </c>
       <c r="D18" t="n">
-        <v>32418.24249649755</v>
+        <v>42344.80885217746</v>
       </c>
       <c r="E18" t="n">
-        <v>-182411.5237049875</v>
+        <v>-341926.6601577442</v>
       </c>
     </row>
     <row r="19">
@@ -4184,16 +4184,16 @@
         <v>37</v>
       </c>
       <c r="B19" t="n">
-        <v>-115702</v>
+        <v>-201176.9999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>-49468.5374848597</v>
+        <v>-119630.8431490862</v>
       </c>
       <c r="D19" t="n">
-        <v>18698.72416465114</v>
+        <v>28625.29052033105</v>
       </c>
       <c r="E19" t="n">
-        <v>-146471.8133202085</v>
+        <v>-292182.5526287551</v>
       </c>
     </row>
     <row r="20">
@@ -4201,16 +4201,16 @@
         <v>38</v>
       </c>
       <c r="B20" t="n">
-        <v>-81671.99999999996</v>
+        <v>-163921.9999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>-33839.30876823427</v>
+        <v>-93422.21728825069</v>
       </c>
       <c r="D20" t="n">
-        <v>8219.829472297673</v>
+        <v>18146.39582797758</v>
       </c>
       <c r="E20" t="n">
-        <v>-107291.4792959366</v>
+        <v>-239197.8214602731</v>
       </c>
     </row>
     <row r="21">
@@ -4218,16 +4218,16 @@
         <v>39</v>
       </c>
       <c r="B21" t="n">
-        <v>-47641.99999999995</v>
+        <v>-126666.9999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>-18210.08005160882</v>
+        <v>-67213.59142741511</v>
       </c>
       <c r="D21" t="n">
-        <v>308.2047397380827</v>
+        <v>10234.77109541799</v>
       </c>
       <c r="E21" t="n">
-        <v>-65543.87531187068</v>
+        <v>-183645.8203319971</v>
       </c>
     </row>
     <row r="22">
@@ -4235,16 +4235,16 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>-13611.99999999995</v>
+        <v>-89411.99999999994</v>
       </c>
       <c r="C22" t="n">
-        <v>-2580.851334983454</v>
+        <v>-41004.96556657969</v>
       </c>
       <c r="D22" t="n">
-        <v>-5601.713382248341</v>
+        <v>4324.852973431564</v>
       </c>
       <c r="E22" t="n">
-        <v>-21794.56471723175</v>
+        <v>-126092.1125931481</v>
       </c>
     </row>
     <row r="23">
@@ -4252,16 +4252,16 @@
         <v>41</v>
       </c>
       <c r="B23" t="n">
-        <v>20418.00000000005</v>
+        <v>-52156.99999999995</v>
       </c>
       <c r="C23" t="n">
-        <v>13048.377381642</v>
+        <v>-14796.33970574412</v>
       </c>
       <c r="D23" t="n">
-        <v>-9972.888297108653</v>
+        <v>-46.321941428748</v>
       </c>
       <c r="E23" t="n">
-        <v>23493.48908453339</v>
+        <v>-66999.6616471728</v>
       </c>
     </row>
     <row r="24">
@@ -4269,16 +4269,16 @@
         <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>54448.00000000005</v>
+        <v>-14901.99999999995</v>
       </c>
       <c r="C24" t="n">
-        <v>28677.6060982674</v>
+        <v>11412.28615509134</v>
       </c>
       <c r="D24" t="n">
-        <v>-13176.2208992239</v>
+        <v>-3249.654543543998</v>
       </c>
       <c r="E24" t="n">
-        <v>69949.38519904355</v>
+        <v>-6739.368388452608</v>
       </c>
     </row>
     <row r="25">
@@ -4286,16 +4286,16 @@
         <v>43</v>
       </c>
       <c r="B25" t="n">
-        <v>88478.00000000004</v>
+        <v>22353.00000000005</v>
       </c>
       <c r="C25" t="n">
-        <v>44306.83481489279</v>
+        <v>37620.91201592685</v>
       </c>
       <c r="D25" t="n">
-        <v>-15503.44737696378</v>
+        <v>-5576.881021283879</v>
       </c>
       <c r="E25" t="n">
-        <v>117281.3874379291</v>
+        <v>54397.03099464303</v>
       </c>
     </row>
     <row r="26">
@@ -4303,16 +4303,16 @@
         <v>44</v>
       </c>
       <c r="B26" t="n">
-        <v>122508</v>
+        <v>59608.00000000005</v>
       </c>
       <c r="C26" t="n">
-        <v>59936.06353151819</v>
+        <v>63829.5378767623</v>
       </c>
       <c r="D26" t="n">
-        <v>-17180.40350805944</v>
+        <v>-7253.837152379537</v>
       </c>
       <c r="E26" t="n">
-        <v>165263.6600234588</v>
+        <v>116183.7007243828</v>
       </c>
     </row>
     <row r="27">
@@ -4320,16 +4320,16 @@
         <v>45</v>
       </c>
       <c r="B27" t="n">
-        <v>156538.0000000001</v>
+        <v>96863.00000000006</v>
       </c>
       <c r="C27" t="n">
-        <v>75565.29224814364</v>
+        <v>90038.16373759788</v>
       </c>
       <c r="D27" t="n">
-        <v>-18379.46278283931</v>
+        <v>-8452.896427159409</v>
       </c>
       <c r="E27" t="n">
-        <v>213723.8294653044</v>
+        <v>178448.2673104385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>